<commit_message>
-Se corrigieron diseños cuando se exportaba durante la aplicacion las facturas
</commit_message>
<xml_diff>
--- a/documents/reports/factura.xlsx
+++ b/documents/reports/factura.xlsx
@@ -74,26 +74,6 @@
       <strike val="false"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="000000"/>
-      <name val="SansSerif"/>
-      <b val="false"/>
-      <i val="false"/>
-      <u val="none"/>
-      <strike val="false"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="000000"/>
-      <name val="Arial"/>
-      <b val="true"/>
-      <i val="false"/>
-      <u val="none"/>
-      <strike val="false"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills>
     <fill>
@@ -226,19 +206,19 @@
       <protection hidden="false" locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <alignment wrapText="true" horizontal="left" vertical="bottom"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <alignment wrapText="true" horizontal="left" vertical="bottom"/>
       <protection hidden="false" locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <alignment wrapText="true" horizontal="left" vertical="bottom"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <alignment wrapText="true" horizontal="left" vertical="bottom"/>
       <protection hidden="false" locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -265,11 +245,11 @@
       <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="12" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="left" vertical="top"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="13" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="13" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="left" vertical="top"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -277,20 +257,20 @@
       <alignment wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="15" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="right" vertical="center"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="16" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="16" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="right" vertical="center"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="17" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="17" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="18" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="18" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="false"/>
     </xf>
   </cellXfs>
@@ -315,35 +295,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="0.16666667"/>
-    <col min="2" max="2" customWidth="1" width="5.1666665"/>
-    <col min="3" max="3" customWidth="1" width="0.16666667"/>
-    <col min="4" max="4" customWidth="1" width="1.5"/>
-    <col min="5" max="5" customWidth="1" width="1.6666666"/>
-    <col min="6" max="6" customWidth="1" width="3.1666667"/>
-    <col min="7" max="7" customWidth="1" width="0.8333333"/>
-    <col min="8" max="8" customWidth="1" width="0.8333333"/>
-    <col min="9" max="9" customWidth="1" width="5.0"/>
-    <col min="10" max="10" customWidth="1" width="10.5"/>
-    <col min="11" max="11" customWidth="1" width="4.5"/>
-    <col min="12" max="12" customWidth="1" width="2.3333333"/>
-    <col min="13" max="13" customWidth="1" width="3.8333333"/>
-    <col min="14" max="14" customWidth="1" width="0.8333333"/>
-    <col min="15" max="15" customWidth="1" width="23.166666"/>
-    <col min="16" max="16" customWidth="1" width="3.1666667"/>
-    <col min="17" max="17" customWidth="1" width="3.8333333"/>
-    <col min="18" max="18" customWidth="1" width="1.0"/>
-    <col min="19" max="19" customWidth="1" width="3.6666667"/>
-    <col min="20" max="20" customWidth="1" width="2.5"/>
-    <col min="21" max="21" customWidth="1" width="2.1666667"/>
-    <col min="22" max="22" customWidth="1" width="1.8333334"/>
-    <col min="23" max="23" customWidth="1" width="9.166667"/>
-    <col min="24" max="24" customWidth="1" width="5.6666665"/>
-    <col min="25" max="25" customWidth="1" width="2.5"/>
-    <col min="26" max="26" customWidth="1" width="0.8333333"/>
+    <col min="1" max="1" customWidth="1" width="5.1666665"/>
+    <col min="2" max="2" customWidth="1" width="0.16666667"/>
+    <col min="3" max="3" customWidth="1" width="0.5"/>
+    <col min="4" max="4" customWidth="1" width="3.6666667"/>
+    <col min="5" max="5" customWidth="1" width="3.0"/>
+    <col min="6" max="6" customWidth="1" width="0.5"/>
+    <col min="7" max="7" customWidth="1" width="5.3333335"/>
+    <col min="8" max="8" customWidth="1" width="10.5"/>
+    <col min="9" max="9" customWidth="1" width="4.5"/>
+    <col min="10" max="10" customWidth="1" width="0.33333334"/>
+    <col min="11" max="11" customWidth="1" width="0.33333334"/>
+    <col min="12" max="12" customWidth="1" width="0.16666667"/>
+    <col min="13" max="13" customWidth="1" width="4.0"/>
+    <col min="14" max="14" customWidth="1" width="1.3333334"/>
+    <col min="15" max="15" customWidth="1" width="1.0"/>
+    <col min="16" max="16" customWidth="1" width="22.666666"/>
+    <col min="17" max="17" customWidth="1" width="0.8333333"/>
+    <col min="18" max="18" customWidth="1" width="4.3333335"/>
+    <col min="19" max="19" customWidth="1" width="2.1666667"/>
+    <col min="20" max="20" customWidth="1" width="1.1666666"/>
+    <col min="21" max="21" customWidth="1" width="3.3333333"/>
+    <col min="22" max="22" customWidth="1" width="4.1666665"/>
+    <col min="23" max="23" customWidth="1" width="0.6666667"/>
+    <col min="24" max="24" customWidth="1" width="1.1666666"/>
+    <col min="25" max="25" customWidth="1" width="4.1666665"/>
+    <col min="26" max="26" customWidth="1" width="5.6666665"/>
+    <col min="27" max="27" customWidth="1" width="0.16666667"/>
+    <col min="28" max="28" customWidth="1" width="3.0"/>
+    <col min="29" max="29" customWidth="1" width="5.0"/>
+    <col min="30" max="30" customWidth="1" width="0.8333333"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" ht="80">
+    <row r="1" customHeight="1" ht="82">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr"/>
       <c r="C1" s="1" t="inlineStr"/>
@@ -370,20 +354,34 @@
       <c r="X1" s="1" t="inlineStr"/>
       <c r="Y1" s="1" t="inlineStr"/>
       <c r="Z1" s="1" t="inlineStr"/>
+      <c r="AA1" s="1" t="inlineStr"/>
+      <c r="AB1" s="1" t="inlineStr"/>
+      <c r="AC1" s="1" t="inlineStr"/>
+      <c r="AD1" s="1" t="inlineStr"/>
     </row>
     <row r="2" customHeight="1" ht="1">
       <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr"/>
-      <c r="C2" s="1" t="inlineStr"/>
-      <c r="D2" s="1" t="inlineStr"/>
-      <c r="E2" s="1" t="inlineStr"/>
-      <c r="F2" s="1" t="inlineStr"/>
-      <c r="G2" s="1" t="inlineStr"/>
-      <c r="H2" s="1" t="inlineStr"/>
-      <c r="I2" s="1" t="inlineStr"/>
-      <c r="J2" s="1" t="inlineStr"/>
-      <c r="K2" s="1" t="inlineStr"/>
-      <c r="L2" s="1" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">CHAU LEGUA CARLOS </t>
+          </r>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr"/>
+      <c r="F2" s="3" t="inlineStr"/>
+      <c r="G2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr"/>
+      <c r="I2" s="3" t="inlineStr"/>
+      <c r="J2" s="3" t="inlineStr"/>
+      <c r="K2" s="3" t="inlineStr"/>
+      <c r="L2" s="3" t="inlineStr"/>
       <c r="M2" s="1" t="inlineStr"/>
       <c r="N2" s="1" t="inlineStr"/>
       <c r="O2" s="1" t="inlineStr"/>
@@ -398,23 +396,17 @@
       <c r="X2" s="1" t="inlineStr"/>
       <c r="Y2" s="1" t="inlineStr"/>
       <c r="Z2" s="1" t="inlineStr"/>
+      <c r="AA2" s="1" t="inlineStr"/>
+      <c r="AB2" s="1" t="inlineStr"/>
+      <c r="AC2" s="1" t="inlineStr"/>
+      <c r="AD2" s="1" t="inlineStr"/>
     </row>
     <row r="3" customHeight="1" ht="12">
       <c r="A3" s="1" t="inlineStr"/>
       <c r="B3" s="1" t="inlineStr"/>
-      <c r="C3" s="1" t="inlineStr"/>
-      <c r="D3" s="1" t="inlineStr"/>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">CHAU LEGUA CARLOS </t>
-          </r>
-        </is>
-      </c>
+      <c r="C3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr"/>
@@ -436,20 +428,24 @@
       <c r="X3" s="1" t="inlineStr"/>
       <c r="Y3" s="1" t="inlineStr"/>
       <c r="Z3" s="1" t="inlineStr"/>
+      <c r="AA3" s="1" t="inlineStr"/>
+      <c r="AB3" s="1" t="inlineStr"/>
+      <c r="AC3" s="1" t="inlineStr"/>
+      <c r="AD3" s="1" t="inlineStr"/>
     </row>
     <row r="4" customHeight="1" ht="1">
       <c r="A4" s="1" t="inlineStr"/>
       <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr"/>
-      <c r="E4" s="3" t="inlineStr"/>
-      <c r="F4" s="3" t="inlineStr"/>
-      <c r="G4" s="3" t="inlineStr"/>
-      <c r="H4" s="3" t="inlineStr"/>
-      <c r="I4" s="3" t="inlineStr"/>
-      <c r="J4" s="3" t="inlineStr"/>
-      <c r="K4" s="3" t="inlineStr"/>
-      <c r="L4" s="3" t="inlineStr"/>
+      <c r="E4" s="1" t="inlineStr"/>
+      <c r="F4" s="1" t="inlineStr"/>
+      <c r="G4" s="1" t="inlineStr"/>
+      <c r="H4" s="1" t="inlineStr"/>
+      <c r="I4" s="1" t="inlineStr"/>
+      <c r="J4" s="1" t="inlineStr"/>
+      <c r="K4" s="1" t="inlineStr"/>
+      <c r="L4" s="1" t="inlineStr"/>
       <c r="M4" s="1" t="inlineStr"/>
       <c r="N4" s="1" t="inlineStr"/>
       <c r="O4" s="1" t="inlineStr"/>
@@ -464,6 +460,10 @@
       <c r="X4" s="1" t="inlineStr"/>
       <c r="Y4" s="1" t="inlineStr"/>
       <c r="Z4" s="1" t="inlineStr"/>
+      <c r="AA4" s="1" t="inlineStr"/>
+      <c r="AB4" s="1" t="inlineStr"/>
+      <c r="AC4" s="1" t="inlineStr"/>
+      <c r="AD4" s="1" t="inlineStr"/>
     </row>
     <row r="5" customHeight="1" ht="10">
       <c r="A5" s="1" t="inlineStr"/>
@@ -492,15 +492,17 @@
       <c r="X5" s="1" t="inlineStr"/>
       <c r="Y5" s="1" t="inlineStr"/>
       <c r="Z5" s="1" t="inlineStr"/>
+      <c r="AA5" s="1" t="inlineStr"/>
+      <c r="AB5" s="1" t="inlineStr"/>
+      <c r="AC5" s="1" t="inlineStr"/>
+      <c r="AD5" s="1" t="inlineStr"/>
     </row>
     <row r="6" customHeight="1" ht="13">
       <c r="A6" s="1" t="inlineStr"/>
       <c r="B6" s="1" t="inlineStr"/>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
-      <c r="E6" s="1" t="inlineStr"/>
-      <c r="F6" s="1" t="inlineStr"/>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -511,13 +513,15 @@
           </r>
         </is>
       </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr"/>
       <c r="I6" s="5" t="inlineStr"/>
       <c r="J6" s="5" t="inlineStr"/>
       <c r="K6" s="5" t="inlineStr"/>
       <c r="L6" s="5" t="inlineStr"/>
       <c r="M6" s="5" t="inlineStr"/>
-      <c r="N6" s="5" t="inlineStr"/>
+      <c r="N6" s="1" t="inlineStr"/>
       <c r="O6" s="1" t="inlineStr"/>
       <c r="P6" s="1" t="inlineStr"/>
       <c r="Q6" s="1" t="inlineStr"/>
@@ -530,8 +534,12 @@
       <c r="X6" s="1" t="inlineStr"/>
       <c r="Y6" s="1" t="inlineStr"/>
       <c r="Z6" s="1" t="inlineStr"/>
-    </row>
-    <row r="7" customHeight="1" ht="14">
+      <c r="AA6" s="1" t="inlineStr"/>
+      <c r="AB6" s="1" t="inlineStr"/>
+      <c r="AC6" s="1" t="inlineStr"/>
+      <c r="AD6" s="1" t="inlineStr"/>
+    </row>
+    <row r="7" customHeight="1" ht="9">
       <c r="A7" s="1" t="inlineStr"/>
       <c r="B7" s="1" t="inlineStr"/>
       <c r="C7" s="1" t="inlineStr"/>
@@ -558,14 +566,16 @@
       <c r="X7" s="1" t="inlineStr"/>
       <c r="Y7" s="1" t="inlineStr"/>
       <c r="Z7" s="1" t="inlineStr"/>
+      <c r="AA7" s="1" t="inlineStr"/>
+      <c r="AB7" s="1" t="inlineStr"/>
+      <c r="AC7" s="1" t="inlineStr"/>
+      <c r="AD7" s="1" t="inlineStr"/>
     </row>
     <row r="8" customHeight="1" ht="14">
       <c r="A8" s="1" t="inlineStr"/>
       <c r="B8" s="1" t="inlineStr"/>
       <c r="C8" s="1" t="inlineStr"/>
-      <c r="D8" s="1" t="inlineStr"/>
-      <c r="E8" s="1" t="inlineStr"/>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -576,6 +586,8 @@
           </r>
         </is>
       </c>
+      <c r="E8" s="3" t="inlineStr"/>
+      <c r="F8" s="3" t="inlineStr"/>
       <c r="G8" s="3" t="inlineStr"/>
       <c r="H8" s="3" t="inlineStr"/>
       <c r="I8" s="3" t="inlineStr"/>
@@ -586,28 +598,52 @@
       <c r="N8" s="3" t="inlineStr"/>
       <c r="O8" s="3" t="inlineStr"/>
       <c r="P8" s="3" t="inlineStr"/>
-      <c r="Q8" s="1" t="inlineStr"/>
+      <c r="Q8" s="3" t="inlineStr"/>
       <c r="R8" s="1" t="inlineStr"/>
-      <c r="S8" s="1" t="inlineStr"/>
-      <c r="T8" s="2" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">29 diciembre 2015</t>
-          </r>
-        </is>
-      </c>
-      <c r="U8" s="3" t="inlineStr"/>
-      <c r="V8" s="3" t="inlineStr"/>
-      <c r="W8" s="3" t="inlineStr"/>
+      <c r="S8" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">29</t>
+          </r>
+        </is>
+      </c>
+      <c r="T8" s="3" t="inlineStr"/>
+      <c r="U8" s="1" t="inlineStr"/>
+      <c r="V8" s="1" t="inlineStr"/>
+      <c r="W8" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">diciembre</t>
+          </r>
+        </is>
+      </c>
       <c r="X8" s="3" t="inlineStr"/>
       <c r="Y8" s="3" t="inlineStr"/>
       <c r="Z8" s="3" t="inlineStr"/>
-    </row>
-    <row r="9" customHeight="1" ht="49">
+      <c r="AA8" s="3" t="inlineStr"/>
+      <c r="AB8" s="1" t="inlineStr"/>
+      <c r="AC8" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">2015</t>
+          </r>
+        </is>
+      </c>
+      <c r="AD8" s="3" t="inlineStr"/>
+    </row>
+    <row r="9" customHeight="1" ht="51">
       <c r="A9" s="1" t="inlineStr"/>
       <c r="B9" s="1" t="inlineStr"/>
       <c r="C9" s="1" t="inlineStr"/>
@@ -634,6 +670,10 @@
       <c r="X9" s="1" t="inlineStr"/>
       <c r="Y9" s="1" t="inlineStr"/>
       <c r="Z9" s="1" t="inlineStr"/>
+      <c r="AA9" s="1" t="inlineStr"/>
+      <c r="AB9" s="1" t="inlineStr"/>
+      <c r="AC9" s="1" t="inlineStr"/>
+      <c r="AD9" s="1" t="inlineStr"/>
     </row>
     <row r="10" customHeight="1" ht="17">
       <c r="A10" s="1" t="inlineStr"/>
@@ -642,9 +682,7 @@
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr"/>
-      <c r="G10" s="1" t="inlineStr"/>
-      <c r="H10" s="1" t="inlineStr"/>
-      <c r="I10" s="6" t="inlineStr">
+      <c r="G10" s="6" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -656,13 +694,15 @@
           </r>
         </is>
       </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
       <c r="K10" s="7" t="inlineStr"/>
       <c r="L10" s="7" t="inlineStr"/>
       <c r="M10" s="7" t="inlineStr"/>
       <c r="N10" s="7" t="inlineStr"/>
       <c r="O10" s="7" t="inlineStr"/>
-      <c r="P10" s="1" t="inlineStr"/>
+      <c r="P10" s="7" t="inlineStr"/>
       <c r="Q10" s="1" t="inlineStr"/>
       <c r="R10" s="1" t="inlineStr"/>
       <c r="S10" s="1" t="inlineStr"/>
@@ -673,38 +713,13 @@
       <c r="X10" s="1" t="inlineStr"/>
       <c r="Y10" s="1" t="inlineStr"/>
       <c r="Z10" s="1" t="inlineStr"/>
-    </row>
-    <row r="11" customHeight="1" ht="7">
-      <c r="A11" s="1" t="inlineStr"/>
-      <c r="B11" s="1" t="inlineStr"/>
-      <c r="C11" s="1" t="inlineStr"/>
-      <c r="D11" s="1" t="inlineStr"/>
-      <c r="E11" s="1" t="inlineStr"/>
-      <c r="F11" s="1" t="inlineStr"/>
-      <c r="G11" s="1" t="inlineStr"/>
-      <c r="H11" s="1" t="inlineStr"/>
-      <c r="I11" s="1" t="inlineStr"/>
-      <c r="J11" s="1" t="inlineStr"/>
-      <c r="K11" s="1" t="inlineStr"/>
-      <c r="L11" s="1" t="inlineStr"/>
-      <c r="M11" s="1" t="inlineStr"/>
-      <c r="N11" s="1" t="inlineStr"/>
-      <c r="O11" s="1" t="inlineStr"/>
-      <c r="P11" s="1" t="inlineStr"/>
-      <c r="Q11" s="1" t="inlineStr"/>
-      <c r="R11" s="1" t="inlineStr"/>
-      <c r="S11" s="1" t="inlineStr"/>
-      <c r="T11" s="1" t="inlineStr"/>
-      <c r="U11" s="1" t="inlineStr"/>
-      <c r="V11" s="1" t="inlineStr"/>
-      <c r="W11" s="1" t="inlineStr"/>
-      <c r="X11" s="1" t="inlineStr"/>
-      <c r="Y11" s="1" t="inlineStr"/>
-      <c r="Z11" s="1" t="inlineStr"/>
-    </row>
-    <row r="12" customHeight="1" ht="16">
-      <c r="A12" s="1" t="inlineStr"/>
-      <c r="B12" s="8" t="inlineStr">
+      <c r="AA10" s="1" t="inlineStr"/>
+      <c r="AB10" s="1" t="inlineStr"/>
+      <c r="AC10" s="1" t="inlineStr"/>
+      <c r="AD10" s="1" t="inlineStr"/>
+    </row>
+    <row r="11" customHeight="1" ht="16">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -716,12 +731,11 @@
           </r>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr"/>
-      <c r="D12" s="9" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr"/>
-      <c r="F12" s="9" t="inlineStr"/>
-      <c r="G12" s="9" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
+      <c r="B11" s="9" t="inlineStr"/>
+      <c r="C11" s="9" t="inlineStr"/>
+      <c r="D11" s="9" t="inlineStr"/>
+      <c r="E11" s="9" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -733,8 +747,8 @@
           </r>
         </is>
       </c>
-      <c r="I12" s="9" t="inlineStr"/>
-      <c r="J12" s="8" t="inlineStr">
+      <c r="G11" s="9" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -746,8 +760,8 @@
           </r>
         </is>
       </c>
-      <c r="K12" s="9" t="inlineStr"/>
-      <c r="L12" s="8" t="inlineStr">
+      <c r="I11" s="9" t="inlineStr"/>
+      <c r="J11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -759,8 +773,11 @@
           </r>
         </is>
       </c>
-      <c r="M12" s="9" t="inlineStr"/>
-      <c r="N12" s="8" t="inlineStr">
+      <c r="K11" s="9" t="inlineStr"/>
+      <c r="L11" s="9" t="inlineStr"/>
+      <c r="M11" s="9" t="inlineStr"/>
+      <c r="N11" s="9" t="inlineStr"/>
+      <c r="O11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -772,10 +789,11 @@
           </r>
         </is>
       </c>
-      <c r="O12" s="9" t="inlineStr"/>
-      <c r="P12" s="9" t="inlineStr"/>
-      <c r="Q12" s="9" t="inlineStr"/>
-      <c r="R12" s="8" t="inlineStr">
+      <c r="P11" s="9" t="inlineStr"/>
+      <c r="Q11" s="9" t="inlineStr"/>
+      <c r="R11" s="9" t="inlineStr"/>
+      <c r="S11" s="9" t="inlineStr"/>
+      <c r="T11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -787,10 +805,10 @@
           </r>
         </is>
       </c>
-      <c r="S12" s="9" t="inlineStr"/>
-      <c r="T12" s="9" t="inlineStr"/>
-      <c r="U12" s="9" t="inlineStr"/>
-      <c r="V12" s="8" t="inlineStr">
+      <c r="U11" s="9" t="inlineStr"/>
+      <c r="V11" s="9" t="inlineStr"/>
+      <c r="W11" s="9" t="inlineStr"/>
+      <c r="X11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -802,8 +820,9 @@
           </r>
         </is>
       </c>
-      <c r="W12" s="9" t="inlineStr"/>
-      <c r="X12" s="8" t="inlineStr">
+      <c r="Y11" s="9" t="inlineStr"/>
+      <c r="Z11" s="9" t="inlineStr"/>
+      <c r="AA11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -815,12 +834,124 @@
           </r>
         </is>
       </c>
-      <c r="Y12" s="9" t="inlineStr"/>
-      <c r="Z12" s="1" t="inlineStr"/>
+      <c r="AB11" s="9" t="inlineStr"/>
+      <c r="AC11" s="9" t="inlineStr"/>
+      <c r="AD11" s="1" t="inlineStr"/>
+    </row>
+    <row r="12" customHeight="1" ht="13">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">27-dic</t>
+          </r>
+        </is>
+      </c>
+      <c r="B12" s="11" t="inlineStr"/>
+      <c r="C12" s="11" t="inlineStr"/>
+      <c r="D12" s="11" t="inlineStr"/>
+      <c r="E12" s="11" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">17:56</t>
+          </r>
+        </is>
+      </c>
+      <c r="G12" s="11" t="inlineStr"/>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">450.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I12" s="11" t="inlineStr"/>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">5</t>
+          </r>
+        </is>
+      </c>
+      <c r="K12" s="11" t="inlineStr"/>
+      <c r="L12" s="11" t="inlineStr"/>
+      <c r="M12" s="11" t="inlineStr"/>
+      <c r="N12" s="11" t="inlineStr"/>
+      <c r="O12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">APTO-LIMA</t>
+          </r>
+        </is>
+      </c>
+      <c r="P12" s="11" t="inlineStr"/>
+      <c r="Q12" s="11" t="inlineStr"/>
+      <c r="R12" s="11" t="inlineStr"/>
+      <c r="S12" s="11" t="inlineStr"/>
+      <c r="T12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">FF-1</t>
+          </r>
+        </is>
+      </c>
+      <c r="U12" s="11" t="inlineStr"/>
+      <c r="V12" s="11" t="inlineStr"/>
+      <c r="W12" s="11" t="inlineStr"/>
+      <c r="X12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">V-01</t>
+          </r>
+        </is>
+      </c>
+      <c r="Y12" s="11" t="inlineStr"/>
+      <c r="Z12" s="11" t="inlineStr"/>
+      <c r="AA12" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">2270.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="AB12" s="11" t="inlineStr"/>
+      <c r="AC12" s="11" t="inlineStr"/>
+      <c r="AD12" s="1" t="inlineStr"/>
     </row>
     <row r="13" customHeight="1" ht="13">
-      <c r="A13" s="1" t="inlineStr"/>
-      <c r="B13" s="10" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -831,10 +962,21 @@
           </r>
         </is>
       </c>
+      <c r="B13" s="11" t="inlineStr"/>
       <c r="C13" s="11" t="inlineStr"/>
       <c r="D13" s="11" t="inlineStr"/>
       <c r="E13" s="11" t="inlineStr"/>
-      <c r="F13" s="11" t="inlineStr"/>
+      <c r="F13" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">18:43</t>
+          </r>
+        </is>
+      </c>
       <c r="G13" s="11" t="inlineStr"/>
       <c r="H13" s="10" t="inlineStr">
         <is>
@@ -843,7 +985,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">17:56</t>
+            <t xml:space="preserve">450.0</t>
           </r>
         </is>
       </c>
@@ -855,38 +997,22 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">450.0</t>
+            <t xml:space="preserve">5</t>
           </r>
         </is>
       </c>
       <c r="K13" s="11" t="inlineStr"/>
-      <c r="L13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">5</t>
-          </r>
-        </is>
-      </c>
+      <c r="L13" s="11" t="inlineStr"/>
       <c r="M13" s="11" t="inlineStr"/>
-      <c r="N13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">APTO-LIMA</t>
-          </r>
-        </is>
-      </c>
-      <c r="O13" s="11" t="inlineStr"/>
+      <c r="N13" s="11" t="inlineStr"/>
+      <c r="O13" s="10" t="inlineStr">
+        <is/>
+      </c>
       <c r="P13" s="11" t="inlineStr"/>
       <c r="Q13" s="11" t="inlineStr"/>
-      <c r="R13" s="10" t="inlineStr">
+      <c r="R13" s="11" t="inlineStr"/>
+      <c r="S13" s="11" t="inlineStr"/>
+      <c r="T13" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -897,20 +1023,8 @@
           </r>
         </is>
       </c>
-      <c r="S13" s="11" t="inlineStr"/>
-      <c r="T13" s="11" t="inlineStr"/>
       <c r="U13" s="11" t="inlineStr"/>
-      <c r="V13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">V-01</t>
-          </r>
-        </is>
-      </c>
+      <c r="V13" s="11" t="inlineStr"/>
       <c r="W13" s="11" t="inlineStr"/>
       <c r="X13" s="10" t="inlineStr">
         <is>
@@ -919,114 +1033,60 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">2270.0</t>
+            <t xml:space="preserve">V-01</t>
           </r>
         </is>
       </c>
       <c r="Y13" s="11" t="inlineStr"/>
-      <c r="Z13" s="1" t="inlineStr"/>
-    </row>
-    <row r="14" customHeight="1" ht="13">
+      <c r="Z13" s="11" t="inlineStr"/>
+      <c r="AA13" s="10" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Arial"/>
+              <sz val="9.0"/>
+            </rPr>
+            <t xml:space="preserve">450.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="AB13" s="11" t="inlineStr"/>
+      <c r="AC13" s="11" t="inlineStr"/>
+      <c r="AD13" s="1" t="inlineStr"/>
+    </row>
+    <row r="14" customHeight="1" ht="213">
       <c r="A14" s="1" t="inlineStr"/>
-      <c r="B14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">27-dic</t>
-          </r>
-        </is>
-      </c>
-      <c r="C14" s="11" t="inlineStr"/>
-      <c r="D14" s="11" t="inlineStr"/>
-      <c r="E14" s="11" t="inlineStr"/>
-      <c r="F14" s="11" t="inlineStr"/>
-      <c r="G14" s="11" t="inlineStr"/>
-      <c r="H14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">18:43</t>
-          </r>
-        </is>
-      </c>
-      <c r="I14" s="11" t="inlineStr"/>
-      <c r="J14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">450.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="K14" s="11" t="inlineStr"/>
-      <c r="L14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">5</t>
-          </r>
-        </is>
-      </c>
-      <c r="M14" s="11" t="inlineStr"/>
-      <c r="N14" s="10" t="inlineStr">
-        <is/>
-      </c>
-      <c r="O14" s="11" t="inlineStr"/>
-      <c r="P14" s="11" t="inlineStr"/>
-      <c r="Q14" s="11" t="inlineStr"/>
-      <c r="R14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">FF-1</t>
-          </r>
-        </is>
-      </c>
-      <c r="S14" s="11" t="inlineStr"/>
-      <c r="T14" s="11" t="inlineStr"/>
-      <c r="U14" s="11" t="inlineStr"/>
-      <c r="V14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">V-01</t>
-          </r>
-        </is>
-      </c>
-      <c r="W14" s="11" t="inlineStr"/>
-      <c r="X14" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">450.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="Y14" s="11" t="inlineStr"/>
+      <c r="B14" s="1" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" s="1" t="inlineStr"/>
+      <c r="E14" s="1" t="inlineStr"/>
+      <c r="F14" s="1" t="inlineStr"/>
+      <c r="G14" s="1" t="inlineStr"/>
+      <c r="H14" s="1" t="inlineStr"/>
+      <c r="I14" s="1" t="inlineStr"/>
+      <c r="J14" s="1" t="inlineStr"/>
+      <c r="K14" s="1" t="inlineStr"/>
+      <c r="L14" s="1" t="inlineStr"/>
+      <c r="M14" s="1" t="inlineStr"/>
+      <c r="N14" s="1" t="inlineStr"/>
+      <c r="O14" s="1" t="inlineStr"/>
+      <c r="P14" s="1" t="inlineStr"/>
+      <c r="Q14" s="1" t="inlineStr"/>
+      <c r="R14" s="1" t="inlineStr"/>
+      <c r="S14" s="1" t="inlineStr"/>
+      <c r="T14" s="1" t="inlineStr"/>
+      <c r="U14" s="1" t="inlineStr"/>
+      <c r="V14" s="1" t="inlineStr"/>
+      <c r="W14" s="1" t="inlineStr"/>
+      <c r="X14" s="1" t="inlineStr"/>
+      <c r="Y14" s="1" t="inlineStr"/>
       <c r="Z14" s="1" t="inlineStr"/>
-    </row>
-    <row r="15" customHeight="1" ht="256">
+      <c r="AA14" s="1" t="inlineStr"/>
+      <c r="AB14" s="1" t="inlineStr"/>
+      <c r="AC14" s="1" t="inlineStr"/>
+      <c r="AD14" s="1" t="inlineStr"/>
+    </row>
+    <row r="15" customHeight="1" ht="14">
       <c r="A15" s="1" t="inlineStr"/>
       <c r="B15" s="1" t="inlineStr"/>
       <c r="C15" s="1" t="inlineStr"/>
@@ -1037,13 +1097,33 @@
       <c r="H15" s="1" t="inlineStr"/>
       <c r="I15" s="1" t="inlineStr"/>
       <c r="J15" s="1" t="inlineStr"/>
-      <c r="K15" s="1" t="inlineStr"/>
-      <c r="L15" s="1" t="inlineStr"/>
-      <c r="M15" s="1" t="inlineStr"/>
-      <c r="N15" s="1" t="inlineStr"/>
-      <c r="O15" s="1" t="inlineStr"/>
-      <c r="P15" s="1" t="inlineStr"/>
-      <c r="Q15" s="1" t="inlineStr"/>
+      <c r="K15" s="12" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">SEDE :</t>
+          </r>
+        </is>
+      </c>
+      <c r="L15" s="13" t="inlineStr"/>
+      <c r="M15" s="13" t="inlineStr"/>
+      <c r="N15" s="13" t="inlineStr"/>
+      <c r="O15" s="13" t="inlineStr"/>
+      <c r="P15" s="12" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">LIMA</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q15" s="13" t="inlineStr"/>
       <c r="R15" s="1" t="inlineStr"/>
       <c r="S15" s="1" t="inlineStr"/>
       <c r="T15" s="1" t="inlineStr"/>
@@ -1053,65 +1133,44 @@
       <c r="X15" s="1" t="inlineStr"/>
       <c r="Y15" s="1" t="inlineStr"/>
       <c r="Z15" s="1" t="inlineStr"/>
+      <c r="AA15" s="1" t="inlineStr"/>
+      <c r="AB15" s="1" t="inlineStr"/>
+      <c r="AC15" s="1" t="inlineStr"/>
+      <c r="AD15" s="1" t="inlineStr"/>
     </row>
     <row r="16" customHeight="1" ht="14">
-      <c r="A16" s="12" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">Sede :</t>
-          </r>
-        </is>
-      </c>
-      <c r="B16" s="13" t="inlineStr"/>
+      <c r="A16" s="1" t="inlineStr"/>
+      <c r="B16" s="1" t="inlineStr"/>
       <c r="C16" s="1" t="inlineStr"/>
-      <c r="D16" s="12" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">LIMA</t>
-          </r>
-        </is>
-      </c>
-      <c r="E16" s="13" t="inlineStr"/>
-      <c r="F16" s="13" t="inlineStr"/>
-      <c r="G16" s="13" t="inlineStr"/>
-      <c r="H16" s="13" t="inlineStr"/>
-      <c r="I16" s="13" t="inlineStr"/>
-      <c r="J16" s="13" t="inlineStr"/>
-      <c r="K16" s="14" t="inlineStr"/>
-      <c r="L16" s="14" t="inlineStr"/>
-      <c r="M16" s="14" t="inlineStr"/>
-      <c r="N16" s="14" t="inlineStr"/>
-      <c r="O16" s="14" t="inlineStr"/>
-      <c r="P16" s="14" t="inlineStr"/>
-      <c r="Q16" s="14" t="inlineStr"/>
-      <c r="R16" s="14" t="inlineStr"/>
-      <c r="S16" s="14" t="inlineStr"/>
-      <c r="T16" s="14" t="inlineStr"/>
-      <c r="U16" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="10.0"/>
-              <b val="true"/>
-            </rPr>
-            <t xml:space="preserve">2720,00</t>
-          </r>
-        </is>
-      </c>
-      <c r="V16" s="16" t="inlineStr"/>
-      <c r="W16" s="16" t="inlineStr"/>
-      <c r="X16" s="16" t="inlineStr"/>
+      <c r="D16" s="1" t="inlineStr"/>
+      <c r="E16" s="1" t="inlineStr"/>
+      <c r="F16" s="1" t="inlineStr"/>
+      <c r="G16" s="1" t="inlineStr"/>
+      <c r="H16" s="1" t="inlineStr"/>
+      <c r="I16" s="1" t="inlineStr"/>
+      <c r="J16" s="1" t="inlineStr"/>
+      <c r="K16" s="1" t="inlineStr"/>
+      <c r="L16" s="1" t="inlineStr"/>
+      <c r="M16" s="1" t="inlineStr"/>
+      <c r="N16" s="1" t="inlineStr"/>
+      <c r="O16" s="1" t="inlineStr"/>
+      <c r="P16" s="1" t="inlineStr"/>
+      <c r="Q16" s="1" t="inlineStr"/>
+      <c r="R16" s="1" t="inlineStr"/>
+      <c r="S16" s="1" t="inlineStr"/>
+      <c r="T16" s="1" t="inlineStr"/>
+      <c r="U16" s="1" t="inlineStr"/>
+      <c r="V16" s="1" t="inlineStr"/>
+      <c r="W16" s="1" t="inlineStr"/>
+      <c r="X16" s="1" t="inlineStr"/>
       <c r="Y16" s="1" t="inlineStr"/>
       <c r="Z16" s="1" t="inlineStr"/>
-    </row>
-    <row r="17" customHeight="1" ht="6">
+      <c r="AA16" s="1" t="inlineStr"/>
+      <c r="AB16" s="1" t="inlineStr"/>
+      <c r="AC16" s="1" t="inlineStr"/>
+      <c r="AD16" s="1" t="inlineStr"/>
+    </row>
+    <row r="17" customHeight="1" ht="11">
       <c r="A17" s="1" t="inlineStr"/>
       <c r="B17" s="1" t="inlineStr"/>
       <c r="C17" s="1" t="inlineStr"/>
@@ -1120,24 +1179,28 @@
       <c r="F17" s="1" t="inlineStr"/>
       <c r="G17" s="1" t="inlineStr"/>
       <c r="H17" s="1" t="inlineStr"/>
-      <c r="I17" s="1" t="inlineStr"/>
-      <c r="J17" s="1" t="inlineStr"/>
+      <c r="I17" s="14" t="inlineStr"/>
+      <c r="J17" s="14" t="inlineStr"/>
       <c r="K17" s="14" t="inlineStr"/>
-      <c r="L17" s="1" t="inlineStr"/>
-      <c r="M17" s="1" t="inlineStr"/>
-      <c r="N17" s="1" t="inlineStr"/>
-      <c r="O17" s="1" t="inlineStr"/>
-      <c r="P17" s="1" t="inlineStr"/>
-      <c r="Q17" s="1" t="inlineStr"/>
-      <c r="R17" s="1" t="inlineStr"/>
-      <c r="S17" s="1" t="inlineStr"/>
-      <c r="T17" s="1" t="inlineStr"/>
-      <c r="U17" s="16" t="inlineStr"/>
-      <c r="V17" s="16" t="inlineStr"/>
-      <c r="W17" s="16" t="inlineStr"/>
-      <c r="X17" s="16" t="inlineStr"/>
-      <c r="Y17" s="1" t="inlineStr"/>
-      <c r="Z17" s="1" t="inlineStr"/>
+      <c r="L17" s="14" t="inlineStr"/>
+      <c r="M17" s="14" t="inlineStr"/>
+      <c r="N17" s="14" t="inlineStr"/>
+      <c r="O17" s="14" t="inlineStr"/>
+      <c r="P17" s="14" t="inlineStr"/>
+      <c r="Q17" s="14" t="inlineStr"/>
+      <c r="R17" s="14" t="inlineStr"/>
+      <c r="S17" s="14" t="inlineStr"/>
+      <c r="T17" s="14" t="inlineStr"/>
+      <c r="U17" s="14" t="inlineStr"/>
+      <c r="V17" s="14" t="inlineStr"/>
+      <c r="W17" s="14" t="inlineStr"/>
+      <c r="X17" s="14" t="inlineStr"/>
+      <c r="Y17" s="14" t="inlineStr"/>
+      <c r="Z17" s="14" t="inlineStr"/>
+      <c r="AA17" s="14" t="inlineStr"/>
+      <c r="AB17" s="14" t="inlineStr"/>
+      <c r="AC17" s="14" t="inlineStr"/>
+      <c r="AD17" s="14" t="inlineStr"/>
     </row>
     <row r="18" customHeight="1" ht="20">
       <c r="A18" s="1" t="inlineStr"/>
@@ -1148,9 +1211,9 @@
       <c r="F18" s="1" t="inlineStr"/>
       <c r="G18" s="1" t="inlineStr"/>
       <c r="H18" s="1" t="inlineStr"/>
-      <c r="I18" s="1" t="inlineStr"/>
+      <c r="I18" s="14" t="inlineStr"/>
       <c r="J18" s="1" t="inlineStr"/>
-      <c r="K18" s="14" t="inlineStr"/>
+      <c r="K18" s="1" t="inlineStr"/>
       <c r="L18" s="1" t="inlineStr"/>
       <c r="M18" s="1" t="inlineStr"/>
       <c r="N18" s="1" t="inlineStr"/>
@@ -1158,35 +1221,28 @@
       <c r="P18" s="1" t="inlineStr"/>
       <c r="Q18" s="1" t="inlineStr"/>
       <c r="R18" s="1" t="inlineStr"/>
-      <c r="S18" s="17" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">IGV 18%</t>
-          </r>
-        </is>
-      </c>
-      <c r="T18" s="18" t="inlineStr"/>
-      <c r="U18" s="18" t="inlineStr"/>
-      <c r="V18" s="18" t="inlineStr"/>
-      <c r="W18" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="10.0"/>
-              <b val="true"/>
-            </rPr>
-            <t xml:space="preserve">489,60</t>
-          </r>
-        </is>
-      </c>
-      <c r="X18" s="16" t="inlineStr"/>
-      <c r="Y18" s="1" t="inlineStr"/>
-      <c r="Z18" s="1" t="inlineStr"/>
+      <c r="S18" s="1" t="inlineStr"/>
+      <c r="T18" s="1" t="inlineStr"/>
+      <c r="U18" s="1" t="inlineStr"/>
+      <c r="V18" s="1" t="inlineStr"/>
+      <c r="W18" s="1" t="inlineStr"/>
+      <c r="X18" s="1" t="inlineStr"/>
+      <c r="Y18" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">2720,00</t>
+          </r>
+        </is>
+      </c>
+      <c r="Z18" s="16" t="inlineStr"/>
+      <c r="AA18" s="16" t="inlineStr"/>
+      <c r="AB18" s="16" t="inlineStr"/>
+      <c r="AC18" s="16" t="inlineStr"/>
+      <c r="AD18" s="16" t="inlineStr"/>
     </row>
     <row r="19" customHeight="1" ht="20">
       <c r="A19" s="1" t="inlineStr"/>
@@ -1197,9 +1253,9 @@
       <c r="F19" s="1" t="inlineStr"/>
       <c r="G19" s="1" t="inlineStr"/>
       <c r="H19" s="1" t="inlineStr"/>
-      <c r="I19" s="1" t="inlineStr"/>
+      <c r="I19" s="14" t="inlineStr"/>
       <c r="J19" s="1" t="inlineStr"/>
-      <c r="K19" s="14" t="inlineStr"/>
+      <c r="K19" s="1" t="inlineStr"/>
       <c r="L19" s="1" t="inlineStr"/>
       <c r="M19" s="1" t="inlineStr"/>
       <c r="N19" s="1" t="inlineStr"/>
@@ -1209,25 +1265,38 @@
       <c r="R19" s="1" t="inlineStr"/>
       <c r="S19" s="1" t="inlineStr"/>
       <c r="T19" s="1" t="inlineStr"/>
-      <c r="U19" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="10.0"/>
-              <b val="true"/>
-            </rPr>
-            <t xml:space="preserve">3209,60</t>
-          </r>
-        </is>
-      </c>
-      <c r="V19" s="16" t="inlineStr"/>
-      <c r="W19" s="16" t="inlineStr"/>
-      <c r="X19" s="16" t="inlineStr"/>
-      <c r="Y19" s="1" t="inlineStr"/>
-      <c r="Z19" s="1" t="inlineStr"/>
-    </row>
-    <row r="20" customHeight="1" ht="25">
+      <c r="U19" s="1" t="inlineStr"/>
+      <c r="V19" s="17" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">IGV 18%</t>
+          </r>
+        </is>
+      </c>
+      <c r="W19" s="18" t="inlineStr"/>
+      <c r="X19" s="18" t="inlineStr"/>
+      <c r="Y19" s="18" t="inlineStr"/>
+      <c r="Z19" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">489,60</t>
+          </r>
+        </is>
+      </c>
+      <c r="AA19" s="16" t="inlineStr"/>
+      <c r="AB19" s="16" t="inlineStr"/>
+      <c r="AC19" s="16" t="inlineStr"/>
+      <c r="AD19" s="16" t="inlineStr"/>
+    </row>
+    <row r="20" customHeight="1" ht="20">
       <c r="A20" s="1" t="inlineStr"/>
       <c r="B20" s="1" t="inlineStr"/>
       <c r="C20" s="1" t="inlineStr"/>
@@ -1236,8 +1305,8 @@
       <c r="F20" s="1" t="inlineStr"/>
       <c r="G20" s="1" t="inlineStr"/>
       <c r="H20" s="1" t="inlineStr"/>
-      <c r="I20" s="1" t="inlineStr"/>
-      <c r="J20" s="1" t="inlineStr"/>
+      <c r="I20" s="14" t="inlineStr"/>
+      <c r="J20" s="14" t="inlineStr"/>
       <c r="K20" s="14" t="inlineStr"/>
       <c r="L20" s="14" t="inlineStr"/>
       <c r="M20" s="14" t="inlineStr"/>
@@ -1252,10 +1321,24 @@
       <c r="V20" s="14" t="inlineStr"/>
       <c r="W20" s="14" t="inlineStr"/>
       <c r="X20" s="14" t="inlineStr"/>
-      <c r="Y20" s="1" t="inlineStr"/>
-      <c r="Z20" s="1" t="inlineStr"/>
-    </row>
-    <row r="21" customHeight="1" ht="99">
+      <c r="Y20" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">3209,60</t>
+          </r>
+        </is>
+      </c>
+      <c r="Z20" s="16" t="inlineStr"/>
+      <c r="AA20" s="16" t="inlineStr"/>
+      <c r="AB20" s="16" t="inlineStr"/>
+      <c r="AC20" s="16" t="inlineStr"/>
+      <c r="AD20" s="16" t="inlineStr"/>
+    </row>
+    <row r="21" customHeight="1" ht="136">
       <c r="A21" s="1" t="inlineStr"/>
       <c r="B21" s="1" t="inlineStr"/>
       <c r="C21" s="1" t="inlineStr"/>
@@ -1282,46 +1365,52 @@
       <c r="X21" s="1" t="inlineStr"/>
       <c r="Y21" s="1" t="inlineStr"/>
       <c r="Z21" s="1" t="inlineStr"/>
+      <c r="AA21" s="1" t="inlineStr"/>
+      <c r="AB21" s="1" t="inlineStr"/>
+      <c r="AC21" s="1" t="inlineStr"/>
+      <c r="AD21" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="E3:L4"/>
-    <mergeCell ref="G6:N6"/>
-    <mergeCell ref="F8:P8"/>
-    <mergeCell ref="T8:Z8"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C2:L3"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="D8:Q8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="W8:AA8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="G10:P10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="O11:S11"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="X12:Y12"/>
-    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="O12:S12"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="R14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="U16:X17"/>
-    <mergeCell ref="S18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="U19:X19"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="O13:S13"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="AA13:AC13"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="Y18:AD18"/>
+    <mergeCell ref="V19:Y19"/>
+    <mergeCell ref="Z19:AD19"/>
+    <mergeCell ref="Y20:AD20"/>
   </mergeCells>
-  <pageMargins left="0.0" right="0.2777777777777778" top="0.625" bottom="0.2777777777777778" header="0.0" footer="0.0"/>
+  <pageMargins left="0.0" right="0.2777777777777778" top="0.6527777777777778" bottom="0.2777777777777778" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rIdDr1"/>
 </worksheet>

</xml_diff>

<commit_message>
-Se agrego el reporte de Ventas -Se corrigio la Columna PAX en el reporte de Files -Se corrigio la lista de ventas, el cual no aparecia la serie de una venta
</commit_message>
<xml_diff>
--- a/documents/reports/factura.xlsx
+++ b/documents/reports/factura.xlsx
@@ -164,16 +164,6 @@
         <fgColor rgb="FFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders>
     <border>
@@ -245,32 +235,24 @@
       <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="13" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="left" vertical="top"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="14" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="13" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="right" vertical="center"/>
+      <alignment wrapText="true" horizontal="center" vertical="bottom"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="16" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="right" vertical="center"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="17" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="18" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
+      <alignment wrapText="true" horizontal="center" vertical="bottom"/>
       <protection hidden="false" locked="false"/>
     </xf>
   </cellXfs>
@@ -327,7 +309,7 @@
     <col min="30" max="30" customWidth="1" width="0.8333333"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" ht="82">
+    <row r="1" customHeight="1" ht="77">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr"/>
       <c r="C1" s="1" t="inlineStr"/>
@@ -576,15 +558,7 @@
       <c r="B8" s="1" t="inlineStr"/>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="2" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">Av.Comandante Espinar 229 Miraflores Lima Lim</t>
-          </r>
-        </is>
+        <is/>
       </c>
       <c r="E8" s="3" t="inlineStr"/>
       <c r="F8" s="3" t="inlineStr"/>
@@ -607,7 +581,7 @@
               <rFont val="Verdana"/>
               <sz val="10.0"/>
             </rPr>
-            <t xml:space="preserve">29</t>
+            <t xml:space="preserve">04</t>
           </r>
         </is>
       </c>
@@ -621,7 +595,7 @@
               <rFont val="Verdana"/>
               <sz val="10.0"/>
             </rPr>
-            <t xml:space="preserve">diciembre</t>
+            <t xml:space="preserve">enero</t>
           </r>
         </is>
       </c>
@@ -637,7 +611,7 @@
               <rFont val="Verdana"/>
               <sz val="10.0"/>
             </rPr>
-            <t xml:space="preserve">2015</t>
+            <t xml:space="preserve">2016</t>
           </r>
         </is>
       </c>
@@ -846,7 +820,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">27-dic</t>
+            <t xml:space="preserve">04-ene</t>
           </r>
         </is>
       </c>
@@ -861,7 +835,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">17:56</t>
+            <t xml:space="preserve">20:14</t>
           </r>
         </is>
       </c>
@@ -873,7 +847,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">450.0</t>
+            <t xml:space="preserve">RTRE-1</t>
           </r>
         </is>
       </c>
@@ -885,7 +859,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -894,15 +868,7 @@
       <c r="M12" s="11" t="inlineStr"/>
       <c r="N12" s="11" t="inlineStr"/>
       <c r="O12" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">APTO-LIMA</t>
-          </r>
-        </is>
+        <is/>
       </c>
       <c r="P12" s="11" t="inlineStr"/>
       <c r="Q12" s="11" t="inlineStr"/>
@@ -915,7 +881,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">FF-1</t>
+            <t xml:space="preserve">F-1</t>
           </r>
         </is>
       </c>
@@ -929,7 +895,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">V-01</t>
+            <t xml:space="preserve">V-09</t>
           </r>
         </is>
       </c>
@@ -942,7 +908,7 @@
               <rFont val="Arial"/>
               <sz val="9.0"/>
             </rPr>
-            <t xml:space="preserve">2270.0</t>
+            <t xml:space="preserve">248.0</t>
           </r>
         </is>
       </c>
@@ -950,111 +916,39 @@
       <c r="AC12" s="11" t="inlineStr"/>
       <c r="AD12" s="1" t="inlineStr"/>
     </row>
-    <row r="13" customHeight="1" ht="13">
-      <c r="A13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">27-dic</t>
-          </r>
-        </is>
-      </c>
-      <c r="B13" s="11" t="inlineStr"/>
-      <c r="C13" s="11" t="inlineStr"/>
-      <c r="D13" s="11" t="inlineStr"/>
-      <c r="E13" s="11" t="inlineStr"/>
-      <c r="F13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">18:43</t>
-          </r>
-        </is>
-      </c>
-      <c r="G13" s="11" t="inlineStr"/>
-      <c r="H13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">450.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="I13" s="11" t="inlineStr"/>
-      <c r="J13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">5</t>
-          </r>
-        </is>
-      </c>
-      <c r="K13" s="11" t="inlineStr"/>
-      <c r="L13" s="11" t="inlineStr"/>
-      <c r="M13" s="11" t="inlineStr"/>
-      <c r="N13" s="11" t="inlineStr"/>
-      <c r="O13" s="10" t="inlineStr">
-        <is/>
-      </c>
-      <c r="P13" s="11" t="inlineStr"/>
-      <c r="Q13" s="11" t="inlineStr"/>
-      <c r="R13" s="11" t="inlineStr"/>
-      <c r="S13" s="11" t="inlineStr"/>
-      <c r="T13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">FF-1</t>
-          </r>
-        </is>
-      </c>
-      <c r="U13" s="11" t="inlineStr"/>
-      <c r="V13" s="11" t="inlineStr"/>
-      <c r="W13" s="11" t="inlineStr"/>
-      <c r="X13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">V-01</t>
-          </r>
-        </is>
-      </c>
-      <c r="Y13" s="11" t="inlineStr"/>
-      <c r="Z13" s="11" t="inlineStr"/>
-      <c r="AA13" s="10" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Arial"/>
-              <sz val="9.0"/>
-            </rPr>
-            <t xml:space="preserve">450.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="AB13" s="11" t="inlineStr"/>
-      <c r="AC13" s="11" t="inlineStr"/>
+    <row r="13" customHeight="1" ht="214">
+      <c r="A13" s="1" t="inlineStr"/>
+      <c r="B13" s="1" t="inlineStr"/>
+      <c r="C13" s="1" t="inlineStr"/>
+      <c r="D13" s="1" t="inlineStr"/>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" s="1" t="inlineStr"/>
+      <c r="G13" s="1" t="inlineStr"/>
+      <c r="H13" s="1" t="inlineStr"/>
+      <c r="I13" s="1" t="inlineStr"/>
+      <c r="J13" s="1" t="inlineStr"/>
+      <c r="K13" s="1" t="inlineStr"/>
+      <c r="L13" s="1" t="inlineStr"/>
+      <c r="M13" s="1" t="inlineStr"/>
+      <c r="N13" s="1" t="inlineStr"/>
+      <c r="O13" s="1" t="inlineStr"/>
+      <c r="P13" s="1" t="inlineStr"/>
+      <c r="Q13" s="1" t="inlineStr"/>
+      <c r="R13" s="1" t="inlineStr"/>
+      <c r="S13" s="1" t="inlineStr"/>
+      <c r="T13" s="1" t="inlineStr"/>
+      <c r="U13" s="1" t="inlineStr"/>
+      <c r="V13" s="1" t="inlineStr"/>
+      <c r="W13" s="1" t="inlineStr"/>
+      <c r="X13" s="1" t="inlineStr"/>
+      <c r="Y13" s="1" t="inlineStr"/>
+      <c r="Z13" s="1" t="inlineStr"/>
+      <c r="AA13" s="1" t="inlineStr"/>
+      <c r="AB13" s="1" t="inlineStr"/>
+      <c r="AC13" s="1" t="inlineStr"/>
       <c r="AD13" s="1" t="inlineStr"/>
     </row>
-    <row r="14" customHeight="1" ht="213">
+    <row r="14" customHeight="1" ht="14">
       <c r="A14" s="1" t="inlineStr"/>
       <c r="B14" s="1" t="inlineStr"/>
       <c r="C14" s="1" t="inlineStr"/>
@@ -1065,13 +959,33 @@
       <c r="H14" s="1" t="inlineStr"/>
       <c r="I14" s="1" t="inlineStr"/>
       <c r="J14" s="1" t="inlineStr"/>
-      <c r="K14" s="1" t="inlineStr"/>
-      <c r="L14" s="1" t="inlineStr"/>
-      <c r="M14" s="1" t="inlineStr"/>
-      <c r="N14" s="1" t="inlineStr"/>
-      <c r="O14" s="1" t="inlineStr"/>
-      <c r="P14" s="1" t="inlineStr"/>
-      <c r="Q14" s="1" t="inlineStr"/>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">SEDE :</t>
+          </r>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr"/>
+      <c r="M14" s="3" t="inlineStr"/>
+      <c r="N14" s="3" t="inlineStr"/>
+      <c r="O14" s="3" t="inlineStr"/>
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">LIMA</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q14" s="3" t="inlineStr"/>
       <c r="R14" s="1" t="inlineStr"/>
       <c r="S14" s="1" t="inlineStr"/>
       <c r="T14" s="1" t="inlineStr"/>
@@ -1086,7 +1000,7 @@
       <c r="AC14" s="1" t="inlineStr"/>
       <c r="AD14" s="1" t="inlineStr"/>
     </row>
-    <row r="15" customHeight="1" ht="14">
+    <row r="15" customHeight="1" ht="12">
       <c r="A15" s="1" t="inlineStr"/>
       <c r="B15" s="1" t="inlineStr"/>
       <c r="C15" s="1" t="inlineStr"/>
@@ -1097,33 +1011,13 @@
       <c r="H15" s="1" t="inlineStr"/>
       <c r="I15" s="1" t="inlineStr"/>
       <c r="J15" s="1" t="inlineStr"/>
-      <c r="K15" s="12" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">SEDE :</t>
-          </r>
-        </is>
-      </c>
-      <c r="L15" s="13" t="inlineStr"/>
-      <c r="M15" s="13" t="inlineStr"/>
-      <c r="N15" s="13" t="inlineStr"/>
-      <c r="O15" s="13" t="inlineStr"/>
-      <c r="P15" s="12" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">LIMA</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q15" s="13" t="inlineStr"/>
+      <c r="K15" s="1" t="inlineStr"/>
+      <c r="L15" s="1" t="inlineStr"/>
+      <c r="M15" s="1" t="inlineStr"/>
+      <c r="N15" s="1" t="inlineStr"/>
+      <c r="O15" s="1" t="inlineStr"/>
+      <c r="P15" s="1" t="inlineStr"/>
+      <c r="Q15" s="1" t="inlineStr"/>
       <c r="R15" s="1" t="inlineStr"/>
       <c r="S15" s="1" t="inlineStr"/>
       <c r="T15" s="1" t="inlineStr"/>
@@ -1138,7 +1032,7 @@
       <c r="AC15" s="1" t="inlineStr"/>
       <c r="AD15" s="1" t="inlineStr"/>
     </row>
-    <row r="16" customHeight="1" ht="14">
+    <row r="16" customHeight="1" ht="20">
       <c r="A16" s="1" t="inlineStr"/>
       <c r="B16" s="1" t="inlineStr"/>
       <c r="C16" s="1" t="inlineStr"/>
@@ -1147,30 +1041,40 @@
       <c r="F16" s="1" t="inlineStr"/>
       <c r="G16" s="1" t="inlineStr"/>
       <c r="H16" s="1" t="inlineStr"/>
-      <c r="I16" s="1" t="inlineStr"/>
-      <c r="J16" s="1" t="inlineStr"/>
-      <c r="K16" s="1" t="inlineStr"/>
-      <c r="L16" s="1" t="inlineStr"/>
-      <c r="M16" s="1" t="inlineStr"/>
-      <c r="N16" s="1" t="inlineStr"/>
-      <c r="O16" s="1" t="inlineStr"/>
-      <c r="P16" s="1" t="inlineStr"/>
-      <c r="Q16" s="1" t="inlineStr"/>
-      <c r="R16" s="1" t="inlineStr"/>
-      <c r="S16" s="1" t="inlineStr"/>
-      <c r="T16" s="1" t="inlineStr"/>
-      <c r="U16" s="1" t="inlineStr"/>
-      <c r="V16" s="1" t="inlineStr"/>
-      <c r="W16" s="1" t="inlineStr"/>
-      <c r="X16" s="1" t="inlineStr"/>
-      <c r="Y16" s="1" t="inlineStr"/>
-      <c r="Z16" s="1" t="inlineStr"/>
-      <c r="AA16" s="1" t="inlineStr"/>
-      <c r="AB16" s="1" t="inlineStr"/>
-      <c r="AC16" s="1" t="inlineStr"/>
-      <c r="AD16" s="1" t="inlineStr"/>
-    </row>
-    <row r="17" customHeight="1" ht="11">
+      <c r="I16" s="12" t="inlineStr"/>
+      <c r="J16" s="12" t="inlineStr"/>
+      <c r="K16" s="12" t="inlineStr"/>
+      <c r="L16" s="12" t="inlineStr"/>
+      <c r="M16" s="12" t="inlineStr"/>
+      <c r="N16" s="12" t="inlineStr"/>
+      <c r="O16" s="12" t="inlineStr"/>
+      <c r="P16" s="12" t="inlineStr"/>
+      <c r="Q16" s="12" t="inlineStr"/>
+      <c r="R16" s="12" t="inlineStr"/>
+      <c r="S16" s="12" t="inlineStr"/>
+      <c r="T16" s="12" t="inlineStr"/>
+      <c r="U16" s="12" t="inlineStr"/>
+      <c r="V16" s="12" t="inlineStr"/>
+      <c r="W16" s="12" t="inlineStr"/>
+      <c r="X16" s="12" t="inlineStr"/>
+      <c r="Y16" s="13" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">248,00</t>
+          </r>
+        </is>
+      </c>
+      <c r="Z16" s="14" t="inlineStr"/>
+      <c r="AA16" s="14" t="inlineStr"/>
+      <c r="AB16" s="14" t="inlineStr"/>
+      <c r="AC16" s="14" t="inlineStr"/>
+      <c r="AD16" s="14" t="inlineStr"/>
+    </row>
+    <row r="17" customHeight="1" ht="20">
       <c r="A17" s="1" t="inlineStr"/>
       <c r="B17" s="1" t="inlineStr"/>
       <c r="C17" s="1" t="inlineStr"/>
@@ -1179,24 +1083,44 @@
       <c r="F17" s="1" t="inlineStr"/>
       <c r="G17" s="1" t="inlineStr"/>
       <c r="H17" s="1" t="inlineStr"/>
-      <c r="I17" s="14" t="inlineStr"/>
-      <c r="J17" s="14" t="inlineStr"/>
-      <c r="K17" s="14" t="inlineStr"/>
-      <c r="L17" s="14" t="inlineStr"/>
-      <c r="M17" s="14" t="inlineStr"/>
-      <c r="N17" s="14" t="inlineStr"/>
-      <c r="O17" s="14" t="inlineStr"/>
-      <c r="P17" s="14" t="inlineStr"/>
-      <c r="Q17" s="14" t="inlineStr"/>
-      <c r="R17" s="14" t="inlineStr"/>
-      <c r="S17" s="14" t="inlineStr"/>
-      <c r="T17" s="14" t="inlineStr"/>
-      <c r="U17" s="14" t="inlineStr"/>
-      <c r="V17" s="14" t="inlineStr"/>
-      <c r="W17" s="14" t="inlineStr"/>
-      <c r="X17" s="14" t="inlineStr"/>
-      <c r="Y17" s="14" t="inlineStr"/>
-      <c r="Z17" s="14" t="inlineStr"/>
+      <c r="I17" s="12" t="inlineStr"/>
+      <c r="J17" s="1" t="inlineStr"/>
+      <c r="K17" s="1" t="inlineStr"/>
+      <c r="L17" s="1" t="inlineStr"/>
+      <c r="M17" s="1" t="inlineStr"/>
+      <c r="N17" s="1" t="inlineStr"/>
+      <c r="O17" s="1" t="inlineStr"/>
+      <c r="P17" s="1" t="inlineStr"/>
+      <c r="Q17" s="1" t="inlineStr"/>
+      <c r="R17" s="1" t="inlineStr"/>
+      <c r="S17" s="1" t="inlineStr"/>
+      <c r="T17" s="1" t="inlineStr"/>
+      <c r="U17" s="1" t="inlineStr"/>
+      <c r="V17" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">IGV 18%</t>
+          </r>
+        </is>
+      </c>
+      <c r="W17" s="16" t="inlineStr"/>
+      <c r="X17" s="16" t="inlineStr"/>
+      <c r="Y17" s="16" t="inlineStr"/>
+      <c r="Z17" s="13" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">44,64</t>
+          </r>
+        </is>
+      </c>
       <c r="AA17" s="14" t="inlineStr"/>
       <c r="AB17" s="14" t="inlineStr"/>
       <c r="AC17" s="14" t="inlineStr"/>
@@ -1211,7 +1135,7 @@
       <c r="F18" s="1" t="inlineStr"/>
       <c r="G18" s="1" t="inlineStr"/>
       <c r="H18" s="1" t="inlineStr"/>
-      <c r="I18" s="14" t="inlineStr"/>
+      <c r="I18" s="12" t="inlineStr"/>
       <c r="J18" s="1" t="inlineStr"/>
       <c r="K18" s="1" t="inlineStr"/>
       <c r="L18" s="1" t="inlineStr"/>
@@ -1227,24 +1151,24 @@
       <c r="V18" s="1" t="inlineStr"/>
       <c r="W18" s="1" t="inlineStr"/>
       <c r="X18" s="1" t="inlineStr"/>
-      <c r="Y18" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">2720,00</t>
-          </r>
-        </is>
-      </c>
-      <c r="Z18" s="16" t="inlineStr"/>
-      <c r="AA18" s="16" t="inlineStr"/>
-      <c r="AB18" s="16" t="inlineStr"/>
-      <c r="AC18" s="16" t="inlineStr"/>
-      <c r="AD18" s="16" t="inlineStr"/>
-    </row>
-    <row r="19" customHeight="1" ht="20">
+      <c r="Y18" s="13" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">292,64</t>
+          </r>
+        </is>
+      </c>
+      <c r="Z18" s="14" t="inlineStr"/>
+      <c r="AA18" s="14" t="inlineStr"/>
+      <c r="AB18" s="14" t="inlineStr"/>
+      <c r="AC18" s="14" t="inlineStr"/>
+      <c r="AD18" s="14" t="inlineStr"/>
+    </row>
+    <row r="19" customHeight="1" ht="25">
       <c r="A19" s="1" t="inlineStr"/>
       <c r="B19" s="1" t="inlineStr"/>
       <c r="C19" s="1" t="inlineStr"/>
@@ -1253,50 +1177,30 @@
       <c r="F19" s="1" t="inlineStr"/>
       <c r="G19" s="1" t="inlineStr"/>
       <c r="H19" s="1" t="inlineStr"/>
-      <c r="I19" s="14" t="inlineStr"/>
-      <c r="J19" s="1" t="inlineStr"/>
-      <c r="K19" s="1" t="inlineStr"/>
-      <c r="L19" s="1" t="inlineStr"/>
-      <c r="M19" s="1" t="inlineStr"/>
-      <c r="N19" s="1" t="inlineStr"/>
-      <c r="O19" s="1" t="inlineStr"/>
-      <c r="P19" s="1" t="inlineStr"/>
-      <c r="Q19" s="1" t="inlineStr"/>
-      <c r="R19" s="1" t="inlineStr"/>
-      <c r="S19" s="1" t="inlineStr"/>
-      <c r="T19" s="1" t="inlineStr"/>
-      <c r="U19" s="1" t="inlineStr"/>
-      <c r="V19" s="17" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">IGV 18%</t>
-          </r>
-        </is>
-      </c>
-      <c r="W19" s="18" t="inlineStr"/>
-      <c r="X19" s="18" t="inlineStr"/>
-      <c r="Y19" s="18" t="inlineStr"/>
-      <c r="Z19" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">489,60</t>
-          </r>
-        </is>
-      </c>
-      <c r="AA19" s="16" t="inlineStr"/>
-      <c r="AB19" s="16" t="inlineStr"/>
-      <c r="AC19" s="16" t="inlineStr"/>
-      <c r="AD19" s="16" t="inlineStr"/>
-    </row>
-    <row r="20" customHeight="1" ht="20">
+      <c r="I19" s="12" t="inlineStr"/>
+      <c r="J19" s="12" t="inlineStr"/>
+      <c r="K19" s="12" t="inlineStr"/>
+      <c r="L19" s="12" t="inlineStr"/>
+      <c r="M19" s="12" t="inlineStr"/>
+      <c r="N19" s="12" t="inlineStr"/>
+      <c r="O19" s="12" t="inlineStr"/>
+      <c r="P19" s="12" t="inlineStr"/>
+      <c r="Q19" s="12" t="inlineStr"/>
+      <c r="R19" s="12" t="inlineStr"/>
+      <c r="S19" s="12" t="inlineStr"/>
+      <c r="T19" s="12" t="inlineStr"/>
+      <c r="U19" s="12" t="inlineStr"/>
+      <c r="V19" s="12" t="inlineStr"/>
+      <c r="W19" s="12" t="inlineStr"/>
+      <c r="X19" s="12" t="inlineStr"/>
+      <c r="Y19" s="12" t="inlineStr"/>
+      <c r="Z19" s="12" t="inlineStr"/>
+      <c r="AA19" s="12" t="inlineStr"/>
+      <c r="AB19" s="12" t="inlineStr"/>
+      <c r="AC19" s="12" t="inlineStr"/>
+      <c r="AD19" s="12" t="inlineStr"/>
+    </row>
+    <row r="20" customHeight="1" ht="141">
       <c r="A20" s="1" t="inlineStr"/>
       <c r="B20" s="1" t="inlineStr"/>
       <c r="C20" s="1" t="inlineStr"/>
@@ -1305,70 +1209,28 @@
       <c r="F20" s="1" t="inlineStr"/>
       <c r="G20" s="1" t="inlineStr"/>
       <c r="H20" s="1" t="inlineStr"/>
-      <c r="I20" s="14" t="inlineStr"/>
-      <c r="J20" s="14" t="inlineStr"/>
-      <c r="K20" s="14" t="inlineStr"/>
-      <c r="L20" s="14" t="inlineStr"/>
-      <c r="M20" s="14" t="inlineStr"/>
-      <c r="N20" s="14" t="inlineStr"/>
-      <c r="O20" s="14" t="inlineStr"/>
-      <c r="P20" s="14" t="inlineStr"/>
-      <c r="Q20" s="14" t="inlineStr"/>
-      <c r="R20" s="14" t="inlineStr"/>
-      <c r="S20" s="14" t="inlineStr"/>
-      <c r="T20" s="14" t="inlineStr"/>
-      <c r="U20" s="14" t="inlineStr"/>
-      <c r="V20" s="14" t="inlineStr"/>
-      <c r="W20" s="14" t="inlineStr"/>
-      <c r="X20" s="14" t="inlineStr"/>
-      <c r="Y20" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">3209,60</t>
-          </r>
-        </is>
-      </c>
-      <c r="Z20" s="16" t="inlineStr"/>
-      <c r="AA20" s="16" t="inlineStr"/>
-      <c r="AB20" s="16" t="inlineStr"/>
-      <c r="AC20" s="16" t="inlineStr"/>
-      <c r="AD20" s="16" t="inlineStr"/>
-    </row>
-    <row r="21" customHeight="1" ht="136">
-      <c r="A21" s="1" t="inlineStr"/>
-      <c r="B21" s="1" t="inlineStr"/>
-      <c r="C21" s="1" t="inlineStr"/>
-      <c r="D21" s="1" t="inlineStr"/>
-      <c r="E21" s="1" t="inlineStr"/>
-      <c r="F21" s="1" t="inlineStr"/>
-      <c r="G21" s="1" t="inlineStr"/>
-      <c r="H21" s="1" t="inlineStr"/>
-      <c r="I21" s="1" t="inlineStr"/>
-      <c r="J21" s="1" t="inlineStr"/>
-      <c r="K21" s="1" t="inlineStr"/>
-      <c r="L21" s="1" t="inlineStr"/>
-      <c r="M21" s="1" t="inlineStr"/>
-      <c r="N21" s="1" t="inlineStr"/>
-      <c r="O21" s="1" t="inlineStr"/>
-      <c r="P21" s="1" t="inlineStr"/>
-      <c r="Q21" s="1" t="inlineStr"/>
-      <c r="R21" s="1" t="inlineStr"/>
-      <c r="S21" s="1" t="inlineStr"/>
-      <c r="T21" s="1" t="inlineStr"/>
-      <c r="U21" s="1" t="inlineStr"/>
-      <c r="V21" s="1" t="inlineStr"/>
-      <c r="W21" s="1" t="inlineStr"/>
-      <c r="X21" s="1" t="inlineStr"/>
-      <c r="Y21" s="1" t="inlineStr"/>
-      <c r="Z21" s="1" t="inlineStr"/>
-      <c r="AA21" s="1" t="inlineStr"/>
-      <c r="AB21" s="1" t="inlineStr"/>
-      <c r="AC21" s="1" t="inlineStr"/>
-      <c r="AD21" s="1" t="inlineStr"/>
+      <c r="I20" s="1" t="inlineStr"/>
+      <c r="J20" s="1" t="inlineStr"/>
+      <c r="K20" s="1" t="inlineStr"/>
+      <c r="L20" s="1" t="inlineStr"/>
+      <c r="M20" s="1" t="inlineStr"/>
+      <c r="N20" s="1" t="inlineStr"/>
+      <c r="O20" s="1" t="inlineStr"/>
+      <c r="P20" s="1" t="inlineStr"/>
+      <c r="Q20" s="1" t="inlineStr"/>
+      <c r="R20" s="1" t="inlineStr"/>
+      <c r="S20" s="1" t="inlineStr"/>
+      <c r="T20" s="1" t="inlineStr"/>
+      <c r="U20" s="1" t="inlineStr"/>
+      <c r="V20" s="1" t="inlineStr"/>
+      <c r="W20" s="1" t="inlineStr"/>
+      <c r="X20" s="1" t="inlineStr"/>
+      <c r="Y20" s="1" t="inlineStr"/>
+      <c r="Z20" s="1" t="inlineStr"/>
+      <c r="AA20" s="1" t="inlineStr"/>
+      <c r="AB20" s="1" t="inlineStr"/>
+      <c r="AC20" s="1" t="inlineStr"/>
+      <c r="AD20" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -1395,22 +1257,14 @@
     <mergeCell ref="T12:W12"/>
     <mergeCell ref="X12:Z12"/>
     <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="O13:S13"/>
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="AA13:AC13"/>
-    <mergeCell ref="K15:O15"/>
-    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="Y16:AD16"/>
+    <mergeCell ref="V17:Y17"/>
+    <mergeCell ref="Z17:AD17"/>
     <mergeCell ref="Y18:AD18"/>
-    <mergeCell ref="V19:Y19"/>
-    <mergeCell ref="Z19:AD19"/>
-    <mergeCell ref="Y20:AD20"/>
   </mergeCells>
-  <pageMargins left="0.0" right="0.2777777777777778" top="0.6527777777777778" bottom="0.2777777777777778" header="0.0" footer="0.0"/>
+  <pageMargins left="0.0" right="0.2777777777777778" top="0.5833333333333334" bottom="0.2777777777777778" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rIdDr1"/>
 </worksheet>

</xml_diff>

<commit_message>
-Se agrego la clase para convertir numeros a letras -Se implemento para los reportes la conversion de numeros a letras
</commit_message>
<xml_diff>
--- a/documents/reports/factura.xlsx
+++ b/documents/reports/factura.xlsx
@@ -164,6 +164,16 @@
         <fgColor rgb="FFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders>
     <border>
@@ -240,18 +250,26 @@
       <protection hidden="false" locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="13" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="left" vertical="center"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="left" vertical="center"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="right" vertical="bottom"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="16" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="right" vertical="bottom"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="17" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="center" vertical="bottom"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="16" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="18" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="center" vertical="bottom"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -284,29 +302,28 @@
     <col min="5" max="5" customWidth="1" width="3.0"/>
     <col min="6" max="6" customWidth="1" width="0.5"/>
     <col min="7" max="7" customWidth="1" width="5.3333335"/>
-    <col min="8" max="8" customWidth="1" width="10.5"/>
-    <col min="9" max="9" customWidth="1" width="4.5"/>
+    <col min="8" max="8" customWidth="1" width="15.0"/>
+    <col min="9" max="9" customWidth="1" width="0.33333334"/>
     <col min="10" max="10" customWidth="1" width="0.33333334"/>
-    <col min="11" max="11" customWidth="1" width="0.33333334"/>
-    <col min="12" max="12" customWidth="1" width="0.16666667"/>
-    <col min="13" max="13" customWidth="1" width="4.0"/>
-    <col min="14" max="14" customWidth="1" width="1.3333334"/>
-    <col min="15" max="15" customWidth="1" width="1.0"/>
-    <col min="16" max="16" customWidth="1" width="22.666666"/>
-    <col min="17" max="17" customWidth="1" width="0.8333333"/>
-    <col min="18" max="18" customWidth="1" width="4.3333335"/>
-    <col min="19" max="19" customWidth="1" width="2.1666667"/>
-    <col min="20" max="20" customWidth="1" width="1.1666666"/>
-    <col min="21" max="21" customWidth="1" width="3.3333333"/>
-    <col min="22" max="22" customWidth="1" width="4.1666665"/>
-    <col min="23" max="23" customWidth="1" width="0.6666667"/>
-    <col min="24" max="24" customWidth="1" width="1.1666666"/>
-    <col min="25" max="25" customWidth="1" width="4.1666665"/>
-    <col min="26" max="26" customWidth="1" width="5.6666665"/>
-    <col min="27" max="27" customWidth="1" width="0.16666667"/>
-    <col min="28" max="28" customWidth="1" width="3.0"/>
-    <col min="29" max="29" customWidth="1" width="5.0"/>
-    <col min="30" max="30" customWidth="1" width="0.8333333"/>
+    <col min="11" max="11" customWidth="1" width="0.16666667"/>
+    <col min="12" max="12" customWidth="1" width="4.0"/>
+    <col min="13" max="13" customWidth="1" width="1.3333334"/>
+    <col min="14" max="14" customWidth="1" width="1.0"/>
+    <col min="15" max="15" customWidth="1" width="22.666666"/>
+    <col min="16" max="16" customWidth="1" width="0.8333333"/>
+    <col min="17" max="17" customWidth="1" width="4.3333335"/>
+    <col min="18" max="18" customWidth="1" width="2.1666667"/>
+    <col min="19" max="19" customWidth="1" width="1.1666666"/>
+    <col min="20" max="20" customWidth="1" width="3.3333333"/>
+    <col min="21" max="21" customWidth="1" width="4.1666665"/>
+    <col min="22" max="22" customWidth="1" width="0.6666667"/>
+    <col min="23" max="23" customWidth="1" width="1.1666666"/>
+    <col min="24" max="24" customWidth="1" width="4.1666665"/>
+    <col min="25" max="25" customWidth="1" width="5.6666665"/>
+    <col min="26" max="26" customWidth="1" width="0.16666667"/>
+    <col min="27" max="27" customWidth="1" width="3.0"/>
+    <col min="28" max="28" customWidth="1" width="5.0"/>
+    <col min="29" max="29" customWidth="1" width="0.8333333"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" ht="77">
@@ -339,7 +356,6 @@
       <c r="AA1" s="1" t="inlineStr"/>
       <c r="AB1" s="1" t="inlineStr"/>
       <c r="AC1" s="1" t="inlineStr"/>
-      <c r="AD1" s="1" t="inlineStr"/>
     </row>
     <row r="2" customHeight="1" ht="1">
       <c r="A2" s="1" t="inlineStr"/>
@@ -363,7 +379,7 @@
       <c r="I2" s="3" t="inlineStr"/>
       <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" s="3" t="inlineStr"/>
-      <c r="L2" s="3" t="inlineStr"/>
+      <c r="L2" s="1" t="inlineStr"/>
       <c r="M2" s="1" t="inlineStr"/>
       <c r="N2" s="1" t="inlineStr"/>
       <c r="O2" s="1" t="inlineStr"/>
@@ -381,7 +397,6 @@
       <c r="AA2" s="1" t="inlineStr"/>
       <c r="AB2" s="1" t="inlineStr"/>
       <c r="AC2" s="1" t="inlineStr"/>
-      <c r="AD2" s="1" t="inlineStr"/>
     </row>
     <row r="3" customHeight="1" ht="12">
       <c r="A3" s="1" t="inlineStr"/>
@@ -395,7 +410,7 @@
       <c r="I3" s="3" t="inlineStr"/>
       <c r="J3" s="3" t="inlineStr"/>
       <c r="K3" s="3" t="inlineStr"/>
-      <c r="L3" s="3" t="inlineStr"/>
+      <c r="L3" s="1" t="inlineStr"/>
       <c r="M3" s="1" t="inlineStr"/>
       <c r="N3" s="1" t="inlineStr"/>
       <c r="O3" s="1" t="inlineStr"/>
@@ -413,7 +428,6 @@
       <c r="AA3" s="1" t="inlineStr"/>
       <c r="AB3" s="1" t="inlineStr"/>
       <c r="AC3" s="1" t="inlineStr"/>
-      <c r="AD3" s="1" t="inlineStr"/>
     </row>
     <row r="4" customHeight="1" ht="1">
       <c r="A4" s="1" t="inlineStr"/>
@@ -445,7 +459,6 @@
       <c r="AA4" s="1" t="inlineStr"/>
       <c r="AB4" s="1" t="inlineStr"/>
       <c r="AC4" s="1" t="inlineStr"/>
-      <c r="AD4" s="1" t="inlineStr"/>
     </row>
     <row r="5" customHeight="1" ht="10">
       <c r="A5" s="1" t="inlineStr"/>
@@ -477,7 +490,6 @@
       <c r="AA5" s="1" t="inlineStr"/>
       <c r="AB5" s="1" t="inlineStr"/>
       <c r="AC5" s="1" t="inlineStr"/>
-      <c r="AD5" s="1" t="inlineStr"/>
     </row>
     <row r="6" customHeight="1" ht="13">
       <c r="A6" s="1" t="inlineStr"/>
@@ -502,7 +514,7 @@
       <c r="J6" s="5" t="inlineStr"/>
       <c r="K6" s="5" t="inlineStr"/>
       <c r="L6" s="5" t="inlineStr"/>
-      <c r="M6" s="5" t="inlineStr"/>
+      <c r="M6" s="1" t="inlineStr"/>
       <c r="N6" s="1" t="inlineStr"/>
       <c r="O6" s="1" t="inlineStr"/>
       <c r="P6" s="1" t="inlineStr"/>
@@ -519,7 +531,6 @@
       <c r="AA6" s="1" t="inlineStr"/>
       <c r="AB6" s="1" t="inlineStr"/>
       <c r="AC6" s="1" t="inlineStr"/>
-      <c r="AD6" s="1" t="inlineStr"/>
     </row>
     <row r="7" customHeight="1" ht="9">
       <c r="A7" s="1" t="inlineStr"/>
@@ -551,7 +562,6 @@
       <c r="AA7" s="1" t="inlineStr"/>
       <c r="AB7" s="1" t="inlineStr"/>
       <c r="AC7" s="1" t="inlineStr"/>
-      <c r="AD7" s="1" t="inlineStr"/>
     </row>
     <row r="8" customHeight="1" ht="14">
       <c r="A8" s="1" t="inlineStr"/>
@@ -572,23 +582,22 @@
       <c r="N8" s="3" t="inlineStr"/>
       <c r="O8" s="3" t="inlineStr"/>
       <c r="P8" s="3" t="inlineStr"/>
-      <c r="Q8" s="3" t="inlineStr"/>
-      <c r="R8" s="1" t="inlineStr"/>
-      <c r="S8" s="2" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">04</t>
-          </r>
-        </is>
-      </c>
-      <c r="T8" s="3" t="inlineStr"/>
+      <c r="Q8" s="1" t="inlineStr"/>
+      <c r="R8" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">13</t>
+          </r>
+        </is>
+      </c>
+      <c r="S8" s="3" t="inlineStr"/>
+      <c r="T8" s="1" t="inlineStr"/>
       <c r="U8" s="1" t="inlineStr"/>
-      <c r="V8" s="1" t="inlineStr"/>
-      <c r="W8" s="2" t="inlineStr">
+      <c r="V8" s="2" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -599,12 +608,12 @@
           </r>
         </is>
       </c>
+      <c r="W8" s="3" t="inlineStr"/>
       <c r="X8" s="3" t="inlineStr"/>
       <c r="Y8" s="3" t="inlineStr"/>
       <c r="Z8" s="3" t="inlineStr"/>
-      <c r="AA8" s="3" t="inlineStr"/>
-      <c r="AB8" s="1" t="inlineStr"/>
-      <c r="AC8" s="2" t="inlineStr">
+      <c r="AA8" s="1" t="inlineStr"/>
+      <c r="AB8" s="2" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -615,7 +624,7 @@
           </r>
         </is>
       </c>
-      <c r="AD8" s="3" t="inlineStr"/>
+      <c r="AC8" s="3" t="inlineStr"/>
     </row>
     <row r="9" customHeight="1" ht="51">
       <c r="A9" s="1" t="inlineStr"/>
@@ -647,7 +656,6 @@
       <c r="AA9" s="1" t="inlineStr"/>
       <c r="AB9" s="1" t="inlineStr"/>
       <c r="AC9" s="1" t="inlineStr"/>
-      <c r="AD9" s="1" t="inlineStr"/>
     </row>
     <row r="10" customHeight="1" ht="17">
       <c r="A10" s="1" t="inlineStr"/>
@@ -676,7 +684,7 @@
       <c r="M10" s="7" t="inlineStr"/>
       <c r="N10" s="7" t="inlineStr"/>
       <c r="O10" s="7" t="inlineStr"/>
-      <c r="P10" s="7" t="inlineStr"/>
+      <c r="P10" s="1" t="inlineStr"/>
       <c r="Q10" s="1" t="inlineStr"/>
       <c r="R10" s="1" t="inlineStr"/>
       <c r="S10" s="1" t="inlineStr"/>
@@ -690,7 +698,6 @@
       <c r="AA10" s="1" t="inlineStr"/>
       <c r="AB10" s="1" t="inlineStr"/>
       <c r="AC10" s="1" t="inlineStr"/>
-      <c r="AD10" s="1" t="inlineStr"/>
     </row>
     <row r="11" customHeight="1" ht="16">
       <c r="A11" s="8" t="inlineStr">
@@ -734,8 +741,7 @@
           </r>
         </is>
       </c>
-      <c r="I11" s="9" t="inlineStr"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -747,11 +753,11 @@
           </r>
         </is>
       </c>
+      <c r="J11" s="9" t="inlineStr"/>
       <c r="K11" s="9" t="inlineStr"/>
       <c r="L11" s="9" t="inlineStr"/>
       <c r="M11" s="9" t="inlineStr"/>
-      <c r="N11" s="9" t="inlineStr"/>
-      <c r="O11" s="8" t="inlineStr">
+      <c r="N11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -763,11 +769,11 @@
           </r>
         </is>
       </c>
+      <c r="O11" s="9" t="inlineStr"/>
       <c r="P11" s="9" t="inlineStr"/>
       <c r="Q11" s="9" t="inlineStr"/>
       <c r="R11" s="9" t="inlineStr"/>
-      <c r="S11" s="9" t="inlineStr"/>
-      <c r="T11" s="8" t="inlineStr">
+      <c r="S11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -779,10 +785,10 @@
           </r>
         </is>
       </c>
+      <c r="T11" s="9" t="inlineStr"/>
       <c r="U11" s="9" t="inlineStr"/>
       <c r="V11" s="9" t="inlineStr"/>
-      <c r="W11" s="9" t="inlineStr"/>
-      <c r="X11" s="8" t="inlineStr">
+      <c r="W11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -794,9 +800,9 @@
           </r>
         </is>
       </c>
+      <c r="X11" s="9" t="inlineStr"/>
       <c r="Y11" s="9" t="inlineStr"/>
-      <c r="Z11" s="9" t="inlineStr"/>
-      <c r="AA11" s="8" t="inlineStr">
+      <c r="Z11" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -804,13 +810,13 @@
               <sz val="10.0"/>
               <u val="single"/>
             </rPr>
-            <t xml:space="preserve">Precio</t>
-          </r>
-        </is>
-      </c>
+            <t xml:space="preserve">US$</t>
+          </r>
+        </is>
+      </c>
+      <c r="AA11" s="9" t="inlineStr"/>
       <c r="AB11" s="9" t="inlineStr"/>
-      <c r="AC11" s="9" t="inlineStr"/>
-      <c r="AD11" s="1" t="inlineStr"/>
+      <c r="AC11" s="1" t="inlineStr"/>
     </row>
     <row r="12" customHeight="1" ht="13">
       <c r="A12" s="10" t="inlineStr">
@@ -851,8 +857,7 @@
           </r>
         </is>
       </c>
-      <c r="I12" s="11" t="inlineStr"/>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="I12" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -863,18 +868,18 @@
           </r>
         </is>
       </c>
+      <c r="J12" s="11" t="inlineStr"/>
       <c r="K12" s="11" t="inlineStr"/>
       <c r="L12" s="11" t="inlineStr"/>
       <c r="M12" s="11" t="inlineStr"/>
-      <c r="N12" s="11" t="inlineStr"/>
-      <c r="O12" s="10" t="inlineStr">
+      <c r="N12" s="10" t="inlineStr">
         <is/>
       </c>
+      <c r="O12" s="11" t="inlineStr"/>
       <c r="P12" s="11" t="inlineStr"/>
       <c r="Q12" s="11" t="inlineStr"/>
       <c r="R12" s="11" t="inlineStr"/>
-      <c r="S12" s="11" t="inlineStr"/>
-      <c r="T12" s="10" t="inlineStr">
+      <c r="S12" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -885,10 +890,10 @@
           </r>
         </is>
       </c>
+      <c r="T12" s="11" t="inlineStr"/>
       <c r="U12" s="11" t="inlineStr"/>
       <c r="V12" s="11" t="inlineStr"/>
-      <c r="W12" s="11" t="inlineStr"/>
-      <c r="X12" s="10" t="inlineStr">
+      <c r="W12" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -899,9 +904,9 @@
           </r>
         </is>
       </c>
+      <c r="X12" s="11" t="inlineStr"/>
       <c r="Y12" s="11" t="inlineStr"/>
-      <c r="Z12" s="11" t="inlineStr"/>
-      <c r="AA12" s="10" t="inlineStr">
+      <c r="Z12" s="10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -912,9 +917,9 @@
           </r>
         </is>
       </c>
+      <c r="AA12" s="11" t="inlineStr"/>
       <c r="AB12" s="11" t="inlineStr"/>
-      <c r="AC12" s="11" t="inlineStr"/>
-      <c r="AD12" s="1" t="inlineStr"/>
+      <c r="AC12" s="1" t="inlineStr"/>
     </row>
     <row r="13" customHeight="1" ht="214">
       <c r="A13" s="1" t="inlineStr"/>
@@ -946,7 +951,6 @@
       <c r="AA13" s="1" t="inlineStr"/>
       <c r="AB13" s="1" t="inlineStr"/>
       <c r="AC13" s="1" t="inlineStr"/>
-      <c r="AD13" s="1" t="inlineStr"/>
     </row>
     <row r="14" customHeight="1" ht="14">
       <c r="A14" s="1" t="inlineStr"/>
@@ -958,8 +962,7 @@
       <c r="G14" s="1" t="inlineStr"/>
       <c r="H14" s="1" t="inlineStr"/>
       <c r="I14" s="1" t="inlineStr"/>
-      <c r="J14" s="1" t="inlineStr"/>
-      <c r="K14" s="2" t="inlineStr">
+      <c r="J14" s="2" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -970,22 +973,23 @@
           </r>
         </is>
       </c>
+      <c r="K14" s="3" t="inlineStr"/>
       <c r="L14" s="3" t="inlineStr"/>
       <c r="M14" s="3" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr"/>
-      <c r="O14" s="3" t="inlineStr"/>
-      <c r="P14" s="2" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">LIMA</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q14" s="3" t="inlineStr"/>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">CUZCO</t>
+          </r>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr"/>
+      <c r="Q14" s="1" t="inlineStr"/>
       <c r="R14" s="1" t="inlineStr"/>
       <c r="S14" s="1" t="inlineStr"/>
       <c r="T14" s="1" t="inlineStr"/>
@@ -998,84 +1002,81 @@
       <c r="AA14" s="1" t="inlineStr"/>
       <c r="AB14" s="1" t="inlineStr"/>
       <c r="AC14" s="1" t="inlineStr"/>
-      <c r="AD14" s="1" t="inlineStr"/>
-    </row>
-    <row r="15" customHeight="1" ht="12">
-      <c r="A15" s="1" t="inlineStr"/>
-      <c r="B15" s="1" t="inlineStr"/>
-      <c r="C15" s="1" t="inlineStr"/>
-      <c r="D15" s="1" t="inlineStr"/>
-      <c r="E15" s="1" t="inlineStr"/>
-      <c r="F15" s="1" t="inlineStr"/>
-      <c r="G15" s="1" t="inlineStr"/>
-      <c r="H15" s="1" t="inlineStr"/>
-      <c r="I15" s="1" t="inlineStr"/>
-      <c r="J15" s="1" t="inlineStr"/>
-      <c r="K15" s="1" t="inlineStr"/>
-      <c r="L15" s="1" t="inlineStr"/>
-      <c r="M15" s="1" t="inlineStr"/>
-      <c r="N15" s="1" t="inlineStr"/>
-      <c r="O15" s="1" t="inlineStr"/>
-      <c r="P15" s="1" t="inlineStr"/>
-      <c r="Q15" s="1" t="inlineStr"/>
-      <c r="R15" s="1" t="inlineStr"/>
-      <c r="S15" s="1" t="inlineStr"/>
-      <c r="T15" s="1" t="inlineStr"/>
-      <c r="U15" s="1" t="inlineStr"/>
-      <c r="V15" s="1" t="inlineStr"/>
-      <c r="W15" s="1" t="inlineStr"/>
-      <c r="X15" s="1" t="inlineStr"/>
-      <c r="Y15" s="1" t="inlineStr"/>
-      <c r="Z15" s="1" t="inlineStr"/>
-      <c r="AA15" s="1" t="inlineStr"/>
-      <c r="AB15" s="1" t="inlineStr"/>
-      <c r="AC15" s="1" t="inlineStr"/>
-      <c r="AD15" s="1" t="inlineStr"/>
+    </row>
+    <row r="15" customHeight="1" ht="2">
+      <c r="A15" s="12" t="inlineStr"/>
+      <c r="B15" s="12" t="inlineStr"/>
+      <c r="C15" s="12" t="inlineStr"/>
+      <c r="D15" s="12" t="inlineStr"/>
+      <c r="E15" s="12" t="inlineStr"/>
+      <c r="F15" s="12" t="inlineStr"/>
+      <c r="G15" s="12" t="inlineStr"/>
+      <c r="H15" s="12" t="inlineStr"/>
+      <c r="I15" s="12" t="inlineStr"/>
+      <c r="J15" s="12" t="inlineStr"/>
+      <c r="K15" s="12" t="inlineStr"/>
+      <c r="L15" s="12" t="inlineStr"/>
+      <c r="M15" s="12" t="inlineStr"/>
+      <c r="N15" s="12" t="inlineStr"/>
+      <c r="O15" s="12" t="inlineStr"/>
+      <c r="P15" s="12" t="inlineStr"/>
+      <c r="Q15" s="12" t="inlineStr"/>
+      <c r="R15" s="12" t="inlineStr"/>
+      <c r="S15" s="12" t="inlineStr"/>
+      <c r="T15" s="12" t="inlineStr"/>
+      <c r="U15" s="12" t="inlineStr"/>
+      <c r="V15" s="12" t="inlineStr"/>
+      <c r="W15" s="12" t="inlineStr"/>
+      <c r="X15" s="12" t="inlineStr"/>
+      <c r="Y15" s="12" t="inlineStr"/>
+      <c r="Z15" s="12" t="inlineStr"/>
+      <c r="AA15" s="12" t="inlineStr"/>
+      <c r="AB15" s="12" t="inlineStr"/>
+      <c r="AC15" s="12" t="inlineStr"/>
     </row>
     <row r="16" customHeight="1" ht="20">
-      <c r="A16" s="1" t="inlineStr"/>
-      <c r="B16" s="1" t="inlineStr"/>
-      <c r="C16" s="1" t="inlineStr"/>
-      <c r="D16" s="1" t="inlineStr"/>
-      <c r="E16" s="1" t="inlineStr"/>
-      <c r="F16" s="1" t="inlineStr"/>
-      <c r="G16" s="1" t="inlineStr"/>
-      <c r="H16" s="1" t="inlineStr"/>
-      <c r="I16" s="12" t="inlineStr"/>
-      <c r="J16" s="12" t="inlineStr"/>
-      <c r="K16" s="12" t="inlineStr"/>
-      <c r="L16" s="12" t="inlineStr"/>
-      <c r="M16" s="12" t="inlineStr"/>
-      <c r="N16" s="12" t="inlineStr"/>
-      <c r="O16" s="12" t="inlineStr"/>
-      <c r="P16" s="12" t="inlineStr"/>
-      <c r="Q16" s="12" t="inlineStr"/>
-      <c r="R16" s="12" t="inlineStr"/>
-      <c r="S16" s="12" t="inlineStr"/>
-      <c r="T16" s="12" t="inlineStr"/>
-      <c r="U16" s="12" t="inlineStr"/>
-      <c r="V16" s="12" t="inlineStr"/>
-      <c r="W16" s="12" t="inlineStr"/>
-      <c r="X16" s="12" t="inlineStr"/>
-      <c r="Y16" s="13" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">248,00</t>
-          </r>
-        </is>
-      </c>
-      <c r="Z16" s="14" t="inlineStr"/>
-      <c r="AA16" s="14" t="inlineStr"/>
-      <c r="AB16" s="14" t="inlineStr"/>
-      <c r="AC16" s="14" t="inlineStr"/>
-      <c r="AD16" s="14" t="inlineStr"/>
+      <c r="A16" s="13" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">SON: DOSCIENTOS NOVENTA Y DOS CON 64/100 DOLARES AMERICANOS</t>
+          </r>
+        </is>
+      </c>
+      <c r="B16" s="14" t="inlineStr"/>
+      <c r="C16" s="14" t="inlineStr"/>
+      <c r="D16" s="14" t="inlineStr"/>
+      <c r="E16" s="14" t="inlineStr"/>
+      <c r="F16" s="14" t="inlineStr"/>
+      <c r="G16" s="14" t="inlineStr"/>
+      <c r="H16" s="14" t="inlineStr"/>
+      <c r="I16" s="14" t="inlineStr"/>
+      <c r="J16" s="14" t="inlineStr"/>
+      <c r="K16" s="14" t="inlineStr"/>
+      <c r="L16" s="14" t="inlineStr"/>
+      <c r="M16" s="14" t="inlineStr"/>
+      <c r="N16" s="14" t="inlineStr"/>
+      <c r="O16" s="14" t="inlineStr"/>
+      <c r="P16" s="14" t="inlineStr"/>
+      <c r="Q16" s="14" t="inlineStr"/>
+      <c r="R16" s="14" t="inlineStr"/>
+      <c r="S16" s="14" t="inlineStr"/>
+      <c r="T16" s="14" t="inlineStr"/>
+      <c r="U16" s="14" t="inlineStr"/>
+      <c r="V16" s="14" t="inlineStr"/>
+      <c r="W16" s="14" t="inlineStr"/>
+      <c r="X16" s="1" t="inlineStr"/>
+      <c r="Y16" s="1" t="inlineStr"/>
+      <c r="Z16" s="1" t="inlineStr"/>
+      <c r="AA16" s="1" t="inlineStr"/>
+      <c r="AB16" s="1" t="inlineStr"/>
+      <c r="AC16" s="12" t="inlineStr"/>
     </row>
     <row r="17" customHeight="1" ht="20">
-      <c r="A17" s="1" t="inlineStr"/>
+      <c r="A17" s="12" t="inlineStr"/>
       <c r="B17" s="1" t="inlineStr"/>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr"/>
@@ -1083,7 +1084,7 @@
       <c r="F17" s="1" t="inlineStr"/>
       <c r="G17" s="1" t="inlineStr"/>
       <c r="H17" s="1" t="inlineStr"/>
-      <c r="I17" s="12" t="inlineStr"/>
+      <c r="I17" s="1" t="inlineStr"/>
       <c r="J17" s="1" t="inlineStr"/>
       <c r="K17" s="1" t="inlineStr"/>
       <c r="L17" s="1" t="inlineStr"/>
@@ -1096,38 +1097,27 @@
       <c r="S17" s="1" t="inlineStr"/>
       <c r="T17" s="1" t="inlineStr"/>
       <c r="U17" s="1" t="inlineStr"/>
-      <c r="V17" s="15" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">IGV 18%</t>
-          </r>
-        </is>
-      </c>
-      <c r="W17" s="16" t="inlineStr"/>
-      <c r="X17" s="16" t="inlineStr"/>
+      <c r="V17" s="1" t="inlineStr"/>
+      <c r="W17" s="1" t="inlineStr"/>
+      <c r="X17" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">248,00</t>
+          </r>
+        </is>
+      </c>
       <c r="Y17" s="16" t="inlineStr"/>
-      <c r="Z17" s="13" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">44,64</t>
-          </r>
-        </is>
-      </c>
-      <c r="AA17" s="14" t="inlineStr"/>
-      <c r="AB17" s="14" t="inlineStr"/>
-      <c r="AC17" s="14" t="inlineStr"/>
-      <c r="AD17" s="14" t="inlineStr"/>
+      <c r="Z17" s="16" t="inlineStr"/>
+      <c r="AA17" s="16" t="inlineStr"/>
+      <c r="AB17" s="16" t="inlineStr"/>
+      <c r="AC17" s="16" t="inlineStr"/>
     </row>
     <row r="18" customHeight="1" ht="20">
-      <c r="A18" s="1" t="inlineStr"/>
+      <c r="A18" s="12" t="inlineStr"/>
       <c r="B18" s="1" t="inlineStr"/>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr"/>
@@ -1135,7 +1125,7 @@
       <c r="F18" s="1" t="inlineStr"/>
       <c r="G18" s="1" t="inlineStr"/>
       <c r="H18" s="1" t="inlineStr"/>
-      <c r="I18" s="12" t="inlineStr"/>
+      <c r="I18" s="1" t="inlineStr"/>
       <c r="J18" s="1" t="inlineStr"/>
       <c r="K18" s="1" t="inlineStr"/>
       <c r="L18" s="1" t="inlineStr"/>
@@ -1147,29 +1137,38 @@
       <c r="R18" s="1" t="inlineStr"/>
       <c r="S18" s="1" t="inlineStr"/>
       <c r="T18" s="1" t="inlineStr"/>
-      <c r="U18" s="1" t="inlineStr"/>
-      <c r="V18" s="1" t="inlineStr"/>
-      <c r="W18" s="1" t="inlineStr"/>
-      <c r="X18" s="1" t="inlineStr"/>
-      <c r="Y18" s="13" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="Verdana"/>
-              <sz val="10.0"/>
-            </rPr>
-            <t xml:space="preserve">292,64</t>
-          </r>
-        </is>
-      </c>
-      <c r="Z18" s="14" t="inlineStr"/>
-      <c r="AA18" s="14" t="inlineStr"/>
-      <c r="AB18" s="14" t="inlineStr"/>
-      <c r="AC18" s="14" t="inlineStr"/>
-      <c r="AD18" s="14" t="inlineStr"/>
-    </row>
-    <row r="19" customHeight="1" ht="25">
-      <c r="A19" s="1" t="inlineStr"/>
+      <c r="U18" s="17" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">      18%</t>
+          </r>
+        </is>
+      </c>
+      <c r="V18" s="18" t="inlineStr"/>
+      <c r="W18" s="18" t="inlineStr"/>
+      <c r="X18" s="18" t="inlineStr"/>
+      <c r="Y18" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">44,64</t>
+          </r>
+        </is>
+      </c>
+      <c r="Z18" s="16" t="inlineStr"/>
+      <c r="AA18" s="16" t="inlineStr"/>
+      <c r="AB18" s="16" t="inlineStr"/>
+      <c r="AC18" s="16" t="inlineStr"/>
+    </row>
+    <row r="19" customHeight="1" ht="20">
+      <c r="A19" s="12" t="inlineStr"/>
       <c r="B19" s="1" t="inlineStr"/>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
@@ -1177,92 +1176,130 @@
       <c r="F19" s="1" t="inlineStr"/>
       <c r="G19" s="1" t="inlineStr"/>
       <c r="H19" s="1" t="inlineStr"/>
-      <c r="I19" s="12" t="inlineStr"/>
-      <c r="J19" s="12" t="inlineStr"/>
-      <c r="K19" s="12" t="inlineStr"/>
-      <c r="L19" s="12" t="inlineStr"/>
-      <c r="M19" s="12" t="inlineStr"/>
-      <c r="N19" s="12" t="inlineStr"/>
-      <c r="O19" s="12" t="inlineStr"/>
-      <c r="P19" s="12" t="inlineStr"/>
-      <c r="Q19" s="12" t="inlineStr"/>
-      <c r="R19" s="12" t="inlineStr"/>
-      <c r="S19" s="12" t="inlineStr"/>
-      <c r="T19" s="12" t="inlineStr"/>
-      <c r="U19" s="12" t="inlineStr"/>
-      <c r="V19" s="12" t="inlineStr"/>
-      <c r="W19" s="12" t="inlineStr"/>
-      <c r="X19" s="12" t="inlineStr"/>
-      <c r="Y19" s="12" t="inlineStr"/>
-      <c r="Z19" s="12" t="inlineStr"/>
-      <c r="AA19" s="12" t="inlineStr"/>
-      <c r="AB19" s="12" t="inlineStr"/>
-      <c r="AC19" s="12" t="inlineStr"/>
-      <c r="AD19" s="12" t="inlineStr"/>
-    </row>
-    <row r="20" customHeight="1" ht="141">
-      <c r="A20" s="1" t="inlineStr"/>
-      <c r="B20" s="1" t="inlineStr"/>
-      <c r="C20" s="1" t="inlineStr"/>
-      <c r="D20" s="1" t="inlineStr"/>
-      <c r="E20" s="1" t="inlineStr"/>
-      <c r="F20" s="1" t="inlineStr"/>
-      <c r="G20" s="1" t="inlineStr"/>
-      <c r="H20" s="1" t="inlineStr"/>
-      <c r="I20" s="1" t="inlineStr"/>
-      <c r="J20" s="1" t="inlineStr"/>
-      <c r="K20" s="1" t="inlineStr"/>
-      <c r="L20" s="1" t="inlineStr"/>
-      <c r="M20" s="1" t="inlineStr"/>
-      <c r="N20" s="1" t="inlineStr"/>
-      <c r="O20" s="1" t="inlineStr"/>
-      <c r="P20" s="1" t="inlineStr"/>
-      <c r="Q20" s="1" t="inlineStr"/>
-      <c r="R20" s="1" t="inlineStr"/>
-      <c r="S20" s="1" t="inlineStr"/>
-      <c r="T20" s="1" t="inlineStr"/>
-      <c r="U20" s="1" t="inlineStr"/>
-      <c r="V20" s="1" t="inlineStr"/>
-      <c r="W20" s="1" t="inlineStr"/>
-      <c r="X20" s="1" t="inlineStr"/>
-      <c r="Y20" s="1" t="inlineStr"/>
-      <c r="Z20" s="1" t="inlineStr"/>
-      <c r="AA20" s="1" t="inlineStr"/>
-      <c r="AB20" s="1" t="inlineStr"/>
-      <c r="AC20" s="1" t="inlineStr"/>
-      <c r="AD20" s="1" t="inlineStr"/>
+      <c r="I19" s="1" t="inlineStr"/>
+      <c r="J19" s="1" t="inlineStr"/>
+      <c r="K19" s="1" t="inlineStr"/>
+      <c r="L19" s="1" t="inlineStr"/>
+      <c r="M19" s="1" t="inlineStr"/>
+      <c r="N19" s="1" t="inlineStr"/>
+      <c r="O19" s="1" t="inlineStr"/>
+      <c r="P19" s="1" t="inlineStr"/>
+      <c r="Q19" s="1" t="inlineStr"/>
+      <c r="R19" s="1" t="inlineStr"/>
+      <c r="S19" s="1" t="inlineStr"/>
+      <c r="T19" s="1" t="inlineStr"/>
+      <c r="U19" s="1" t="inlineStr"/>
+      <c r="V19" s="1" t="inlineStr"/>
+      <c r="W19" s="1" t="inlineStr"/>
+      <c r="X19" s="15" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Verdana"/>
+              <sz val="10.0"/>
+            </rPr>
+            <t xml:space="preserve">292,64</t>
+          </r>
+        </is>
+      </c>
+      <c r="Y19" s="16" t="inlineStr"/>
+      <c r="Z19" s="16" t="inlineStr"/>
+      <c r="AA19" s="16" t="inlineStr"/>
+      <c r="AB19" s="16" t="inlineStr"/>
+      <c r="AC19" s="16" t="inlineStr"/>
+    </row>
+    <row r="20" customHeight="1" ht="23">
+      <c r="A20" s="12" t="inlineStr"/>
+      <c r="B20" s="12" t="inlineStr"/>
+      <c r="C20" s="12" t="inlineStr"/>
+      <c r="D20" s="12" t="inlineStr"/>
+      <c r="E20" s="12" t="inlineStr"/>
+      <c r="F20" s="12" t="inlineStr"/>
+      <c r="G20" s="12" t="inlineStr"/>
+      <c r="H20" s="12" t="inlineStr"/>
+      <c r="I20" s="12" t="inlineStr"/>
+      <c r="J20" s="12" t="inlineStr"/>
+      <c r="K20" s="12" t="inlineStr"/>
+      <c r="L20" s="12" t="inlineStr"/>
+      <c r="M20" s="12" t="inlineStr"/>
+      <c r="N20" s="12" t="inlineStr"/>
+      <c r="O20" s="12" t="inlineStr"/>
+      <c r="P20" s="12" t="inlineStr"/>
+      <c r="Q20" s="12" t="inlineStr"/>
+      <c r="R20" s="12" t="inlineStr"/>
+      <c r="S20" s="12" t="inlineStr"/>
+      <c r="T20" s="12" t="inlineStr"/>
+      <c r="U20" s="12" t="inlineStr"/>
+      <c r="V20" s="12" t="inlineStr"/>
+      <c r="W20" s="12" t="inlineStr"/>
+      <c r="X20" s="12" t="inlineStr"/>
+      <c r="Y20" s="12" t="inlineStr"/>
+      <c r="Z20" s="12" t="inlineStr"/>
+      <c r="AA20" s="12" t="inlineStr"/>
+      <c r="AB20" s="12" t="inlineStr"/>
+      <c r="AC20" s="12" t="inlineStr"/>
+    </row>
+    <row r="21" customHeight="1" ht="133">
+      <c r="A21" s="1" t="inlineStr"/>
+      <c r="B21" s="1" t="inlineStr"/>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="inlineStr"/>
+      <c r="E21" s="1" t="inlineStr"/>
+      <c r="F21" s="1" t="inlineStr"/>
+      <c r="G21" s="1" t="inlineStr"/>
+      <c r="H21" s="1" t="inlineStr"/>
+      <c r="I21" s="1" t="inlineStr"/>
+      <c r="J21" s="1" t="inlineStr"/>
+      <c r="K21" s="1" t="inlineStr"/>
+      <c r="L21" s="1" t="inlineStr"/>
+      <c r="M21" s="1" t="inlineStr"/>
+      <c r="N21" s="1" t="inlineStr"/>
+      <c r="O21" s="1" t="inlineStr"/>
+      <c r="P21" s="1" t="inlineStr"/>
+      <c r="Q21" s="1" t="inlineStr"/>
+      <c r="R21" s="1" t="inlineStr"/>
+      <c r="S21" s="1" t="inlineStr"/>
+      <c r="T21" s="1" t="inlineStr"/>
+      <c r="U21" s="1" t="inlineStr"/>
+      <c r="V21" s="1" t="inlineStr"/>
+      <c r="W21" s="1" t="inlineStr"/>
+      <c r="X21" s="1" t="inlineStr"/>
+      <c r="Y21" s="1" t="inlineStr"/>
+      <c r="Z21" s="1" t="inlineStr"/>
+      <c r="AA21" s="1" t="inlineStr"/>
+      <c r="AB21" s="1" t="inlineStr"/>
+      <c r="AC21" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="C2:L3"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="D8:Q8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="W8:AA8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="G10:P10"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="D8:P8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="V8:Z8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="G10:O10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="S11:V11"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="O12:S12"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="Y16:AD16"/>
-    <mergeCell ref="V17:Y17"/>
-    <mergeCell ref="Z17:AD17"/>
-    <mergeCell ref="Y18:AD18"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="Z12:AB12"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A16:W16"/>
+    <mergeCell ref="X17:AC17"/>
+    <mergeCell ref="U18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="X19:AC19"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.2777777777777778" top="0.5833333333333334" bottom="0.2777777777777778" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>